<commit_message>
Finalised crop wild relatives checklist template. Working on taxon distribution template schema.
</commit_message>
<xml_diff>
--- a/Library/snippets/CWR_Checklist_Template.xlsx
+++ b/Library/snippets/CWR_Checklist_Template.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-33220" yWindow="780" windowWidth="25540" windowHeight="17300" tabRatio="724" activeTab="2"/>
+    <workbookView xWindow="-33220" yWindow="780" windowWidth="25540" windowHeight="17300" tabRatio="724" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Read this" sheetId="13" r:id="rId1"/>
     <sheet name="CK_Identification" sheetId="10" r:id="rId2"/>
     <sheet name="CK_Crossability" sheetId="11" r:id="rId3"/>
-    <sheet name="TEMP_Threatened status (3)" sheetId="12" r:id="rId4"/>
+    <sheet name="CK_Threats" sheetId="12" r:id="rId4"/>
     <sheet name="List code and descriptions" sheetId="7" r:id="rId5"/>
   </sheets>
   <definedNames>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="394">
   <si>
     <t xml:space="preserve">Country code identifying the National CWR checklist; the code of the country preparing the CWR checklist. For country codes use the three-letter ISO 3166-1 (see: http://unstats.un.org/unsd/methods/m49/m49alpha.htm ) </t>
   </si>
@@ -974,176 +974,176 @@
     <t xml:space="preserve">3.3. Economic Value of the Related Crop </t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">3.2.1. Period of occurrence of threat </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
+    <t>CK :KINGDOM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CK:NUMB </t>
+  </si>
+  <si>
+    <t>CK:INSTCODE</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CK:TYPE</t>
+  </si>
+  <si>
+    <t>CK:REF</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CK:TAXONID</t>
+  </si>
+  <si>
+    <t>CK :PHYLUM/DIVISION</t>
+  </si>
+  <si>
+    <t>CK :CLASS</t>
+  </si>
+  <si>
+    <t>CK :ORDER</t>
+  </si>
+  <si>
+    <t>CK:FAMILY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CK:GENUS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CK:SPECIES </t>
+  </si>
+  <si>
+    <t>CK:SPAUTHOR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CK:SUBTAXON </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CK:SUBTAUTHOR </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CK:TAXREF </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CK:TAXREFID </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CK:SYNONYMS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CK:SYNREF </t>
+  </si>
+  <si>
+    <t>CK:COMMONTAXONNAME</t>
+  </si>
+  <si>
+    <t>CK:LANGCOMMONTAXONNAME</t>
+  </si>
+  <si>
+    <t>CK:CHROMOSNUMB</t>
+  </si>
+  <si>
+    <t>CK:GENEPOOL</t>
+  </si>
+  <si>
+    <t>CK:TAXONGROUP</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CK:GENEPOOLREF</t>
+  </si>
+  <si>
+    <t>CK: REFTAXONGROUP</t>
+  </si>
+  <si>
+    <t>CK:CROSS</t>
+  </si>
+  <si>
+    <t>CK:LISTSPCROSS</t>
+  </si>
+  <si>
+    <t>CK:LISTSPCROSSREF</t>
+  </si>
+  <si>
+    <t>CK:METHCROSSREF</t>
+  </si>
+  <si>
+    <t>CK:SUCCROSSREF</t>
+  </si>
+  <si>
+    <t>CK:THREATSTATUS</t>
+  </si>
+  <si>
+    <t>CK:ASSLEVEL</t>
+  </si>
+  <si>
+    <t>CK:REGIONASS</t>
+  </si>
+  <si>
+    <t>CK:IUCNCAT</t>
+  </si>
+  <si>
+    <t>CK:IUCNCRIT</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CK:REDLISTCAT</t>
+  </si>
+  <si>
+    <t>CK:URLPUBREDLISTASS</t>
+  </si>
+  <si>
+    <t>CK:REFREDLISTASS</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CK:TAXONSTATUS</t>
+  </si>
+  <si>
+    <t>CK:IUCNTHREATCLSS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CK:OCCURTHREAT </t>
+  </si>
+  <si>
+    <t>CK:ECOVALUE</t>
+  </si>
+  <si>
+    <t>CK:ECOVALUEREF</t>
+  </si>
+  <si>
+    <t>CK:URL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.20.3. List of species crosses references </t>
+  </si>
+  <si>
+    <t>0. Unique identifier-</t>
+  </si>
+  <si>
+    <t>CK (CK_UNID)*</t>
+  </si>
+  <si>
+    <t>Checklist identification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.20.2. Method(s) used for crosses </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Describe the method9s) used for each identified crosses. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Multiple values are separated by semicolon </t>
+    </r>
+    <r>
+      <rPr>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t/>
-    </r>
-  </si>
-  <si>
-    <t>CK :KINGDOM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CK:NUMB </t>
-  </si>
-  <si>
-    <t>CK:INSTCODE</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> CK:TYPE</t>
-  </si>
-  <si>
-    <t>CK:REF</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> CK:TAXONID</t>
-  </si>
-  <si>
-    <t>CK :PHYLUM/DIVISION</t>
-  </si>
-  <si>
-    <t>CK :CLASS</t>
-  </si>
-  <si>
-    <t>CK :ORDER</t>
-  </si>
-  <si>
-    <t>CK:FAMILY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CK:GENUS </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CK:SPECIES </t>
-  </si>
-  <si>
-    <t>CK:SPAUTHOR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CK:SUBTAXON </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CK:SUBTAUTHOR </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CK:TAXREF </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CK:TAXREFID </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CK:SYNONYMS </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CK:SYNREF </t>
-  </si>
-  <si>
-    <t>CK:COMMONTAXONNAME</t>
-  </si>
-  <si>
-    <t>CK:LANGCOMMONTAXONNAME</t>
-  </si>
-  <si>
-    <t>CK:CHROMOSNUMB</t>
-  </si>
-  <si>
-    <t>CK:GENEPOOL</t>
-  </si>
-  <si>
-    <t>CK:TAXONGROUP</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> CK:GENEPOOLREF</t>
-  </si>
-  <si>
-    <t>CK: REFTAXONGROUP</t>
-  </si>
-  <si>
-    <t>CK:CROSS</t>
-  </si>
-  <si>
-    <t>CK:LISTSPCROSS</t>
-  </si>
-  <si>
-    <t>CK:LISTSPCROSSREF</t>
-  </si>
-  <si>
-    <t>CK:METHCROSSREF</t>
-  </si>
-  <si>
-    <t>CK:SUCCROSSREF</t>
-  </si>
-  <si>
-    <t>CK:THREATSTATUS</t>
-  </si>
-  <si>
-    <t>CK:ASSLEVEL</t>
-  </si>
-  <si>
-    <t>CK:REGIONASS</t>
-  </si>
-  <si>
-    <t>CK:IUCNCAT</t>
-  </si>
-  <si>
-    <t>CK:IUCNCRIT</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> CK:REDLISTCAT</t>
-  </si>
-  <si>
-    <t>CK:URLPUBREDLISTASS</t>
-  </si>
-  <si>
-    <t>CK:REFREDLISTASS</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> CK:TAXONSTATUS</t>
-  </si>
-  <si>
-    <t>CK:IUCNTHREATCLSS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CK:OCCURTHREAT </t>
-  </si>
-  <si>
-    <t>CK:ECOVALUE</t>
-  </si>
-  <si>
-    <t>CK:ECOVALUEREF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.1.3. IUCN Red List Category IUCN Red List Categories and Criteria Version 3.1: IUCN, 2001, http://www.iucnredlist.org/static/categories:criteria:3:1.  IUCN Red List Category of the taxon </t>
-  </si>
-  <si>
-    <t>CK:URL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.20.3. List of species crosses references </t>
-  </si>
-  <si>
-    <t>0. Unique identifier-</t>
-  </si>
-  <si>
-    <t>CK (CK_UNID)*</t>
-  </si>
-  <si>
-    <t>Checklist identification</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.20.2. Method(s) used for crosses </t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Describe the method9s) used for each identified crosses. </t>
+      <t xml:space="preserve">(;) </t>
     </r>
     <r>
       <rPr>
@@ -1152,48 +1152,30 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">Multiple values are separated by semicolon </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">(;) </t>
-    </r>
-    <r>
-      <rPr>
+      <t>without space.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Provide the language of the common taxon name (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>without space.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Provide the language of the common taxon name (</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
+      <t>Standard: ISO 639-2</t>
+    </r>
+    <r>
+      <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>Standard: ISO 639-2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
       <t xml:space="preserve">) and the name of the taxon in colloquial language. Separate sub elements with @ and multiple elements by semicolon (;) without space. Use ISO 639-2, alpha-3 in Codes for the representation of name languages (see: http//www.loc.gov/standards/iso639-2/php/code_list.php)  </t>
     </r>
   </si>
@@ -1213,18 +1195,12 @@
     <t xml:space="preserve">2.18. Taxon Group </t>
   </si>
   <si>
-    <t>CK:UNID*</t>
-  </si>
-  <si>
     <t>SHEET1</t>
   </si>
   <si>
     <t>0. Unique identifier</t>
   </si>
   <si>
-    <t>Threatened Status</t>
-  </si>
-  <si>
     <t xml:space="preserve">Field specific for uniquely identify your cwr checklist. The combination you provide must  be in unique for each row on the first column of the excel template. This column is fixed and this ID must be the same for the “Crossbaility and “Threatened status” sheets of this checklist.  </t>
   </si>
   <si>
@@ -1277,9 +1253,6 @@
   </si>
   <si>
     <t>Dataset name, provide the dataset or collection name to which this entry belongs.</t>
-  </si>
-  <si>
-    <t>DATASET</t>
   </si>
   <si>
     <t xml:space="preserve">National CWR checklist code </t>
@@ -1492,24 +1465,6 @@
   </si>
   <si>
     <t>CK_TYPE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">References </t>
-  </si>
-  <si>
-    <t>Any bibliographic references related to the publication of the checklist, the format should include the author, date, title, journal, volume and page number or the DOI number, multiple entries should be separated by a semicolon (;)</t>
-  </si>
-  <si>
-    <t>REFERENCE</t>
-  </si>
-  <si>
-    <t>URL link</t>
-  </si>
-  <si>
-    <t>URL linking to any additional data about the checklist species either in the institute or from another source.</t>
-  </si>
-  <si>
-    <t>URL</t>
   </si>
   <si>
     <t xml:space="preserve">Kingdom </t>
@@ -1807,12 +1762,402 @@
   <si>
     <t>VERSION</t>
   </si>
+  <si>
+    <t>DATASET_NAME</t>
+  </si>
+  <si>
+    <t>DATASET_URL</t>
+  </si>
+  <si>
+    <t>Dataset report</t>
+  </si>
+  <si>
+    <t>Provide the URLs pointing to the reports or sources of the dataset, separate multiple entries with a semicolon (;).</t>
+  </si>
+  <si>
+    <t>DATASET_NOTES</t>
+  </si>
+  <si>
+    <t>Provide dataset notes or comments.</t>
+  </si>
+  <si>
+    <t>Dataset notes</t>
+  </si>
+  <si>
+    <t>INVENTORY_CODE</t>
+  </si>
+  <si>
+    <t>Inventory code</t>
+  </si>
+  <si>
+    <t>Provide the unique code identifying the inventory, if available and relevant.</t>
+  </si>
+  <si>
+    <t>Inventory administrative unit</t>
+  </si>
+  <si>
+    <t>INVENTORY_ADMINISTRATIVE_UNIT</t>
+  </si>
+  <si>
+    <t>Provide the geographical administrative unit related to the inventory, this may be a country or a country subdivision. For country codes use the three-letter ISO 3166-1 Alpha-3 code; for region codes use the ISO 3166-2 codes (see: http://en.wikipedia.org/wiki/ISO_3166-1).</t>
+  </si>
+  <si>
+    <t>Inventory institute</t>
+  </si>
+  <si>
+    <t>INVENTORY_INSTCODE</t>
+  </si>
+  <si>
+    <t>Provide the FAO/WIEWS institute code of the responsible organisation. The codes consist of the 3 letter ISO 3166 country code of the country where the institute is located plus a number. The current set of institute codes is available from http://apps3.fao.org/wiews/wiews.jsp</t>
+  </si>
+  <si>
+    <t>References</t>
+  </si>
+  <si>
+    <t>REFERENCES</t>
+  </si>
+  <si>
+    <t>Provide any bibliographic references related to the publication, the format should include the author, date, title, journal, volume and page number or the DOI number; multiple entries should be separated by a semicolon (;).</t>
+  </si>
+  <si>
+    <t>Links</t>
+  </si>
+  <si>
+    <t>URLS</t>
+  </si>
+  <si>
+    <t>Provide any internet links (URL) holding any additional data either in the institute or from another source; ; multiple entries should be separated by a semicolon (;).</t>
+  </si>
+  <si>
+    <t>Field specific for uniquely identifying your cwr checklist. The value you provide must reference the CK_UNID column in the CK_Identification worksheet whose row corresponds to the checklist featuring this crossability record.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List of species crosses </t>
+  </si>
+  <si>
+    <t>LISTSPCROSS</t>
+  </si>
+  <si>
+    <t>List the species that have been crossed, separated the items by semicolons (;) without space.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Method(s) used for crosses </t>
+  </si>
+  <si>
+    <t>METHCROSSREF</t>
+  </si>
+  <si>
+    <t>Describe the method(s) used for each identified crosses. Multiple values are separated by semicolon (;) without space.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">List of species crosses references </t>
+  </si>
+  <si>
+    <t>LISTSPCROSSREF</t>
+  </si>
+  <si>
+    <t>Add bibliographic references related to the species crossed, the format should include the author, date, title, journal, volume and page number or the DOI number. Multiple values are separated by semicolon (;) without space.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Success rate of crosses </t>
+  </si>
+  <si>
+    <t>SUCCROSSREF</t>
+  </si>
+  <si>
+    <t>Indicate the percentage (%) of success rate for each cross. Multiple values are separated by semicolon (;) without space.</t>
+  </si>
+  <si>
+    <t>Population type</t>
+  </si>
+  <si>
+    <t>POPCROSSREF</t>
+  </si>
+  <si>
+    <t>Indicate the type of cross population.</t>
+  </si>
+  <si>
+    <t>Crossability</t>
+  </si>
+  <si>
+    <t>This worksheet contains the crossability data.</t>
+  </si>
+  <si>
+    <t>Threats</t>
+  </si>
+  <si>
+    <t>This worksheet contains the species threats status data.</t>
+  </si>
+  <si>
+    <t>Field specific for uniquely identifying your cwr checklist. The value you provide must reference the CK_UNID column in the CK_Identification worksheet whose row corresponds to the checklist featuring this threat status record.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Red List assessment level </t>
+  </si>
+  <si>
+    <t>ASSESSMENT_LEVEL</t>
+  </si>
+  <si>
+    <t>Indicate level of Red List assessment:
+1: Global
+2: Regional
+3: National</t>
+  </si>
+  <si>
+    <t>Example 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Region of assessment </t>
+  </si>
+  <si>
+    <t>ASSESSMENT_REGION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IUCN Red List Category </t>
+  </si>
+  <si>
+    <t>Indicate the IUCN Red List Category (IUCN Red List Categories and Criteria Version 3.1: IUCN, 2001), http://www.iucnredlist.org/static/categories_criteria_3_1):
+CR: Critically endangered
+DD: Data deficiency
+EN: Endangered
+EW: Extinct in the wild
+EX: Extinct
+LC: Least concern
+NE: Not evaluated
+NT: Near threatened
+VU: Vulnerable
+LR/cd: Lower risk: conservation dependent
+LR/nt: Lower risk: near threatened
+LR/lc: Lower risk: least concern</t>
+  </si>
+  <si>
+    <t>Example: EN</t>
+  </si>
+  <si>
+    <t>IUCN Red List Criteria</t>
+  </si>
+  <si>
+    <t>Indicate the IUCN Red List Criteria (IUCN Red List Categories and Criteria Version 3.1: IUCN, 2001), http://www.iucnredlist.org/static/categories_criteria_3_1):
+A: Declining population
+B: Geographic range size
+C: Small population size
+D: Very small population
+E: Quantitative analysis of extinction risk</t>
+  </si>
+  <si>
+    <t>Example: A</t>
+  </si>
+  <si>
+    <t>IUCN Red List Citation</t>
+  </si>
+  <si>
+    <t>For the categories CR, EN and VU, for which criteria and subcriteria are an integral part of the Red List assessment, provide the IUCN criteria and subcriteria that apply to the taxon as a result of the Red listing process in the standard format,  (see Annex I), e.g. B2ab(iii) IUCN 2012b.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other Red List categories and criteria </t>
+  </si>
+  <si>
+    <t>IUCN_CATEGORY</t>
+  </si>
+  <si>
+    <t>IUCN_CRITERIA</t>
+  </si>
+  <si>
+    <t>IUCN_CITATION</t>
+  </si>
+  <si>
+    <t>OTHER_CRITERIA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IUCN threat classification </t>
+  </si>
+  <si>
+    <t>IUCN_THREAT</t>
+  </si>
+  <si>
+    <t>Indicate the IUCN Red List Threat Category (IUCN Threats Classification Scheme: http://www.iucnredlist.org/technical-documents/classification-schemes/threats-classification-scheme).</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Example: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">2.1.1 </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>= Shifting agriculture</t>
+    </r>
+  </si>
+  <si>
+    <t>THREAT_PERIOD</t>
+  </si>
+  <si>
+    <t>Indicate the threat period of occurrence:
+1: Past
+2: Present
+3: Future</t>
+  </si>
+  <si>
+    <t>Example: 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Year of IUCN Red List assessment </t>
+  </si>
+  <si>
+    <t>ASSESSMENT_YEAR</t>
+  </si>
+  <si>
+    <t>Provide the year in which Red List assessment was carried out.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">URL publication details of Red List assessment </t>
+  </si>
+  <si>
+    <t>ASSESSMENT_URL</t>
+  </si>
+  <si>
+    <t>Provide URL linking to the additional Red List assessment publication details.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">References details of Red List assessment </t>
+  </si>
+  <si>
+    <t>ASSESSMENT_REFERENCES</t>
+  </si>
+  <si>
+    <t>Any bibliographic references related to the publication of the checklist, the format should include the author, date, title, journal, volume and page number or the DOI number, multiple entries should be separated by a semicolon (;).</t>
+  </si>
+  <si>
+    <t>NatureServe global ranking</t>
+  </si>
+  <si>
+    <t>Indicate the taxon threat global ranking (NatureServe 2009):
+GX: Known or presumed extinct in the wild
+G1: Globally critically imperiled
+G2: Globally imperiled
+G3: Globally vulnerable
+G4: Apparently secure
+G5: Apparently secure and globally secure</t>
+  </si>
+  <si>
+    <t>Example: G3</t>
+  </si>
+  <si>
+    <t>NATSERVE_RANKING</t>
+  </si>
+  <si>
+    <t>Threaten status according to national criteria</t>
+  </si>
+  <si>
+    <t>Provide threaten status according to national criteria.</t>
+  </si>
+  <si>
+    <t>THREAT_NATIONAL</t>
+  </si>
+  <si>
+    <t>National unit code</t>
+  </si>
+  <si>
+    <t>Provide threaten national unit code.</t>
+  </si>
+  <si>
+    <t>THREAT_NATIONAL_UCODE</t>
+  </si>
+  <si>
+    <t>National unit description</t>
+  </si>
+  <si>
+    <t>THREAT_NATIONAL_UDESCR</t>
+  </si>
+  <si>
+    <t>Provide threaten national unit description.</t>
+  </si>
+  <si>
+    <t>National unit authority</t>
+  </si>
+  <si>
+    <t>THREAT_NATIONAL_UAUTH</t>
+  </si>
+  <si>
+    <t>Provide threaten national unit authority.</t>
+  </si>
+  <si>
+    <t>Year of national red list assessment</t>
+  </si>
+  <si>
+    <t>THREAT_NATIONAL_YEAR</t>
+  </si>
+  <si>
+    <t>Provide year of national red list assessment.</t>
+  </si>
+  <si>
+    <t>Taxon occurrence status</t>
+  </si>
+  <si>
+    <t>Indication of the status of the taxon in the country (TDWG-POSS):
+100: Native
+110: Endemic
+120: Indigenous
+130: Assumed to be native
+200: Doubtfully native
+300: Formerly native (extinct)
+400: Non native
+410: Transient
+420: Naturalised
+430: Adventive
+490: Recorded as native in error</t>
+  </si>
+  <si>
+    <t>OCCURRENCE_STATUS</t>
+  </si>
+  <si>
+    <t>Threat occurrence notes</t>
+  </si>
+  <si>
+    <t>OCCURRENCE_NOTES</t>
+  </si>
+  <si>
+    <t>Provide notes or comments on occurrence.</t>
+  </si>
+  <si>
+    <t>Example: 120</t>
+  </si>
+  <si>
+    <r>
+      <t>Period of occurrence of threat</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="30" x14ac:knownFonts="1">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1937,13 +2282,6 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Palatino"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -2200,97 +2538,115 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="88">
+  <cellStyleXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -2339,25 +2695,10 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -2381,60 +2722,39 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2442,21 +2762,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2465,16 +2785,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="26" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2484,13 +2804,39 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="88">
+  <cellStyles count="106">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -2534,6 +2880,15 @@
     <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="91" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="93" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
@@ -2578,6 +2933,15 @@
     <cellStyle name="Hyperlink" xfId="82" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="84" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="86" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="88" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="90" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="92" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="94" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="96" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="98" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="100" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="102" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="104" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3993,667 +4357,730 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:AO9"/>
+  <dimension ref="A1:AS8"/>
   <sheetViews>
-    <sheetView topLeftCell="AM1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:AN8"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="40.1640625" style="35" customWidth="1"/>
-    <col min="2" max="40" width="40.1640625" style="36" customWidth="1"/>
-    <col min="41" max="41" width="8.83203125" style="36"/>
-    <col min="42" max="16384" width="8.83203125" style="37"/>
+    <col min="1" max="1" width="39.5" style="8" customWidth="1"/>
+    <col min="2" max="30" width="39.5" style="25" customWidth="1"/>
+    <col min="31" max="45" width="39.5" customWidth="1"/>
+    <col min="46" max="16384" width="8.83203125" style="27"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" s="42" customFormat="1" ht="18">
-      <c r="A1" s="58" t="s">
-        <v>148</v>
-      </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59"/>
-      <c r="J1" s="59"/>
-      <c r="K1" s="59"/>
-      <c r="L1" s="59"/>
-      <c r="M1" s="59"/>
-      <c r="N1" s="59"/>
-      <c r="O1" s="59"/>
-      <c r="P1" s="59"/>
-      <c r="Q1" s="59"/>
-      <c r="R1" s="59"/>
-      <c r="S1" s="59"/>
-      <c r="T1" s="59"/>
-      <c r="U1" s="59"/>
-      <c r="V1" s="59"/>
-      <c r="W1" s="59"/>
-      <c r="X1" s="59"/>
-      <c r="Y1" s="59"/>
-      <c r="Z1" s="59"/>
-      <c r="AA1" s="59"/>
-      <c r="AB1" s="59"/>
-      <c r="AC1" s="59"/>
-      <c r="AD1" s="59"/>
-      <c r="AE1" s="59"/>
-      <c r="AF1" s="59"/>
-      <c r="AG1" s="59"/>
-      <c r="AH1" s="59"/>
-      <c r="AI1" s="59"/>
-      <c r="AJ1" s="59"/>
-      <c r="AK1" s="59"/>
-      <c r="AL1" s="59"/>
-      <c r="AM1" s="59"/>
-      <c r="AN1" s="60"/>
-      <c r="AO1" s="41"/>
-    </row>
-    <row r="2" spans="1:41" s="44" customFormat="1" ht="15">
-      <c r="A2" s="61" t="s">
+    <row r="1" spans="1:45" s="30" customFormat="1" ht="18">
+      <c r="A1" s="44" t="s">
+        <v>146</v>
+      </c>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
+      <c r="N1" s="45"/>
+      <c r="O1" s="45"/>
+      <c r="P1" s="45"/>
+      <c r="Q1" s="45"/>
+      <c r="R1" s="45"/>
+      <c r="S1" s="45"/>
+      <c r="T1" s="45"/>
+      <c r="U1" s="45"/>
+      <c r="V1" s="45"/>
+      <c r="W1" s="45"/>
+      <c r="X1" s="45"/>
+      <c r="Y1" s="45"/>
+      <c r="Z1" s="45"/>
+      <c r="AA1" s="45"/>
+      <c r="AB1" s="45"/>
+      <c r="AC1" s="45"/>
+      <c r="AD1" s="45"/>
+      <c r="AE1" s="45"/>
+      <c r="AF1" s="45"/>
+      <c r="AG1" s="45"/>
+      <c r="AH1" s="45"/>
+      <c r="AI1" s="45"/>
+      <c r="AJ1" s="45"/>
+      <c r="AK1" s="45"/>
+      <c r="AL1" s="45"/>
+      <c r="AM1" s="45"/>
+      <c r="AN1" s="45"/>
+      <c r="AO1" s="45"/>
+      <c r="AP1" s="45"/>
+      <c r="AQ1" s="45"/>
+      <c r="AR1" s="45"/>
+      <c r="AS1" s="46"/>
+    </row>
+    <row r="2" spans="1:45" s="32" customFormat="1" ht="15">
+      <c r="A2" s="47" t="s">
+        <v>169</v>
+      </c>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="31"/>
+      <c r="P2" s="31"/>
+      <c r="Q2" s="31"/>
+      <c r="R2" s="31"/>
+      <c r="S2" s="31"/>
+      <c r="T2" s="31"/>
+      <c r="U2" s="31"/>
+      <c r="V2" s="31"/>
+      <c r="W2" s="31"/>
+      <c r="X2" s="31"/>
+      <c r="Y2" s="31"/>
+      <c r="Z2" s="31"/>
+      <c r="AA2" s="31"/>
+      <c r="AB2" s="31"/>
+      <c r="AC2" s="31"/>
+      <c r="AD2" s="31"/>
+      <c r="AE2" s="31"/>
+      <c r="AF2" s="31"/>
+      <c r="AG2" s="31"/>
+      <c r="AH2" s="31"/>
+      <c r="AI2" s="31"/>
+      <c r="AJ2" s="31"/>
+      <c r="AK2" s="31"/>
+      <c r="AL2" s="31"/>
+      <c r="AM2" s="31"/>
+      <c r="AN2" s="31"/>
+      <c r="AO2" s="31"/>
+      <c r="AP2" s="31"/>
+      <c r="AQ2" s="31"/>
+      <c r="AR2" s="31"/>
+      <c r="AS2" s="48"/>
+    </row>
+    <row r="3" spans="1:45" s="32" customFormat="1" ht="15">
+      <c r="A3" s="47"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="31"/>
+      <c r="N3" s="31"/>
+      <c r="O3" s="31"/>
+      <c r="P3" s="31"/>
+      <c r="Q3" s="31"/>
+      <c r="R3" s="31"/>
+      <c r="S3" s="31"/>
+      <c r="T3" s="31"/>
+      <c r="U3" s="31"/>
+      <c r="V3" s="31"/>
+      <c r="W3" s="31"/>
+      <c r="X3" s="31"/>
+      <c r="Y3" s="31"/>
+      <c r="Z3" s="31"/>
+      <c r="AA3" s="31"/>
+      <c r="AB3" s="31"/>
+      <c r="AC3" s="31"/>
+      <c r="AD3" s="31"/>
+      <c r="AE3" s="31"/>
+      <c r="AF3" s="31"/>
+      <c r="AG3" s="31"/>
+      <c r="AH3" s="31"/>
+      <c r="AI3" s="31"/>
+      <c r="AJ3" s="31"/>
+      <c r="AK3" s="31"/>
+      <c r="AL3" s="31"/>
+      <c r="AM3" s="31"/>
+      <c r="AN3" s="31"/>
+      <c r="AO3" s="31"/>
+      <c r="AP3" s="31"/>
+      <c r="AQ3" s="31"/>
+      <c r="AR3" s="31"/>
+      <c r="AS3" s="48"/>
+    </row>
+    <row r="4" spans="1:45" s="33" customFormat="1">
+      <c r="A4" s="49" t="s">
+        <v>170</v>
+      </c>
+      <c r="B4" s="39" t="s">
         <v>173</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="43"/>
-      <c r="L2" s="43"/>
-      <c r="M2" s="43"/>
-      <c r="N2" s="43"/>
-      <c r="O2" s="43"/>
-      <c r="P2" s="43"/>
-      <c r="Q2" s="43"/>
-      <c r="R2" s="43"/>
-      <c r="S2" s="43"/>
-      <c r="T2" s="43"/>
-      <c r="U2" s="43"/>
-      <c r="V2" s="43"/>
-      <c r="W2" s="43"/>
-      <c r="X2" s="43"/>
-      <c r="Y2" s="43"/>
-      <c r="Z2" s="43"/>
-      <c r="AA2" s="43"/>
-      <c r="AB2" s="43"/>
-      <c r="AC2" s="43"/>
-      <c r="AD2" s="43"/>
-      <c r="AE2" s="43"/>
-      <c r="AF2" s="43"/>
-      <c r="AG2" s="43"/>
-      <c r="AH2" s="43"/>
-      <c r="AI2" s="43"/>
-      <c r="AJ2" s="43"/>
-      <c r="AK2" s="43"/>
-      <c r="AL2" s="43"/>
-      <c r="AM2" s="43"/>
-      <c r="AN2" s="62"/>
-      <c r="AO2" s="43"/>
-    </row>
-    <row r="3" spans="1:41" s="44" customFormat="1" ht="15">
-      <c r="A3" s="61"/>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
-      <c r="K3" s="43"/>
-      <c r="L3" s="43"/>
-      <c r="M3" s="43"/>
-      <c r="N3" s="43"/>
-      <c r="O3" s="43"/>
-      <c r="P3" s="43"/>
-      <c r="Q3" s="43"/>
-      <c r="R3" s="43"/>
-      <c r="S3" s="43"/>
-      <c r="T3" s="43"/>
-      <c r="U3" s="43"/>
-      <c r="V3" s="43"/>
-      <c r="W3" s="43"/>
-      <c r="X3" s="43"/>
-      <c r="Y3" s="43"/>
-      <c r="Z3" s="43"/>
-      <c r="AA3" s="43"/>
-      <c r="AB3" s="43"/>
-      <c r="AC3" s="43"/>
-      <c r="AD3" s="43"/>
-      <c r="AE3" s="43"/>
-      <c r="AF3" s="43"/>
-      <c r="AG3" s="43"/>
-      <c r="AH3" s="43"/>
-      <c r="AI3" s="43"/>
-      <c r="AJ3" s="43"/>
-      <c r="AK3" s="43"/>
-      <c r="AL3" s="43"/>
-      <c r="AM3" s="43"/>
-      <c r="AN3" s="62"/>
-      <c r="AO3" s="43"/>
-    </row>
-    <row r="4" spans="1:41" s="46" customFormat="1">
-      <c r="A4" s="63" t="s">
+      <c r="C4" s="39" t="s">
+        <v>291</v>
+      </c>
+      <c r="D4" s="39" t="s">
+        <v>295</v>
+      </c>
+      <c r="E4" s="39" t="s">
+        <v>297</v>
+      </c>
+      <c r="F4" s="39" t="s">
+        <v>299</v>
+      </c>
+      <c r="G4" s="39" t="s">
+        <v>302</v>
+      </c>
+      <c r="H4" s="39" t="s">
+        <v>305</v>
+      </c>
+      <c r="I4" s="39" t="s">
+        <v>308</v>
+      </c>
+      <c r="J4" s="39" t="s">
+        <v>189</v>
+      </c>
+      <c r="K4" s="66" t="s">
+        <v>175</v>
+      </c>
+      <c r="L4" s="66" t="s">
+        <v>180</v>
+      </c>
+      <c r="M4" s="67" t="s">
+        <v>187</v>
+      </c>
+      <c r="N4" s="67" t="s">
+        <v>191</v>
+      </c>
+      <c r="O4" s="65" t="s">
+        <v>194</v>
+      </c>
+      <c r="P4" s="65" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q4" s="65" t="s">
+        <v>202</v>
+      </c>
+      <c r="R4" s="65" t="s">
+        <v>204</v>
+      </c>
+      <c r="S4" s="65" t="s">
+        <v>205</v>
+      </c>
+      <c r="T4" s="65" t="s">
+        <v>208</v>
+      </c>
+      <c r="U4" s="65" t="s">
+        <v>212</v>
+      </c>
+      <c r="V4" s="65" t="s">
+        <v>215</v>
+      </c>
+      <c r="W4" s="65" t="s">
+        <v>219</v>
+      </c>
+      <c r="X4" s="65" t="s">
+        <v>223</v>
+      </c>
+      <c r="Y4" s="65" t="s">
+        <v>196</v>
+      </c>
+      <c r="Z4" s="65" t="s">
+        <v>261</v>
+      </c>
+      <c r="AA4" s="65" t="s">
+        <v>228</v>
+      </c>
+      <c r="AB4" s="65" t="s">
+        <v>231</v>
+      </c>
+      <c r="AC4" s="65" t="s">
+        <v>234</v>
+      </c>
+      <c r="AD4" s="65" t="s">
+        <v>237</v>
+      </c>
+      <c r="AE4" s="65" t="s">
+        <v>241</v>
+      </c>
+      <c r="AF4" s="65" t="s">
+        <v>243</v>
+      </c>
+      <c r="AG4" s="65" t="s">
+        <v>246</v>
+      </c>
+      <c r="AH4" s="65" t="s">
+        <v>248</v>
+      </c>
+      <c r="AI4" s="65" t="s">
+        <v>250</v>
+      </c>
+      <c r="AJ4" s="65" t="s">
+        <v>265</v>
+      </c>
+      <c r="AK4" s="65" t="s">
+        <v>268</v>
+      </c>
+      <c r="AL4" s="65" t="s">
+        <v>275</v>
+      </c>
+      <c r="AM4" s="65" t="s">
+        <v>271</v>
+      </c>
+      <c r="AN4" s="65" t="s">
+        <v>279</v>
+      </c>
+      <c r="AO4" s="65" t="s">
+        <v>282</v>
+      </c>
+      <c r="AP4" s="65" t="s">
+        <v>285</v>
+      </c>
+      <c r="AQ4" s="65" t="s">
+        <v>252</v>
+      </c>
+      <c r="AR4" s="66" t="s">
+        <v>255</v>
+      </c>
+      <c r="AS4" s="68" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="5" spans="1:45" s="28" customFormat="1" ht="154">
+      <c r="A5" s="50" t="s">
+        <v>171</v>
+      </c>
+      <c r="B5" s="41" t="s">
         <v>174</v>
       </c>
-      <c r="B4" s="52" t="s">
+      <c r="C5" s="41" t="s">
+        <v>292</v>
+      </c>
+      <c r="D5" s="41" t="s">
+        <v>294</v>
+      </c>
+      <c r="E5" s="41" t="s">
+        <v>298</v>
+      </c>
+      <c r="F5" s="41" t="s">
+        <v>301</v>
+      </c>
+      <c r="G5" s="41" t="s">
+        <v>304</v>
+      </c>
+      <c r="H5" s="41" t="s">
+        <v>307</v>
+      </c>
+      <c r="I5" s="41" t="s">
+        <v>310</v>
+      </c>
+      <c r="J5" s="41" t="s">
+        <v>190</v>
+      </c>
+      <c r="K5" s="41" t="s">
         <v>177</v>
       </c>
-      <c r="C4" s="52" t="s">
-        <v>194</v>
-      </c>
-      <c r="D4" s="53" t="s">
-        <v>180</v>
-      </c>
-      <c r="E4" s="53" t="s">
+      <c r="L5" s="42" t="s">
+        <v>181</v>
+      </c>
+      <c r="M5" s="42" t="s">
+        <v>188</v>
+      </c>
+      <c r="N5" s="40" t="s">
+        <v>192</v>
+      </c>
+      <c r="O5" s="34"/>
+      <c r="P5" s="34"/>
+      <c r="Q5" s="34"/>
+      <c r="R5" s="34"/>
+      <c r="S5" s="34"/>
+      <c r="T5" s="34" t="s">
+        <v>210</v>
+      </c>
+      <c r="U5" s="34" t="s">
+        <v>213</v>
+      </c>
+      <c r="V5" s="34" t="s">
+        <v>216</v>
+      </c>
+      <c r="W5" s="34" t="s">
+        <v>220</v>
+      </c>
+      <c r="X5" s="43" t="s">
+        <v>225</v>
+      </c>
+      <c r="Y5" s="34" t="s">
+        <v>197</v>
+      </c>
+      <c r="Z5" s="34" t="s">
+        <v>262</v>
+      </c>
+      <c r="AA5" s="34" t="s">
+        <v>229</v>
+      </c>
+      <c r="AB5" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC5" s="34" t="s">
+        <v>236</v>
+      </c>
+      <c r="AD5" s="34" t="s">
+        <v>239</v>
+      </c>
+      <c r="AE5" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF5" s="34" t="s">
+        <v>245</v>
+      </c>
+      <c r="AG5" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH5" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="AI5" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ5" s="34" t="s">
+        <v>266</v>
+      </c>
+      <c r="AK5" s="34" t="s">
+        <v>269</v>
+      </c>
+      <c r="AL5" s="34" t="s">
+        <v>276</v>
+      </c>
+      <c r="AM5" s="34" t="s">
+        <v>273</v>
+      </c>
+      <c r="AN5" s="34" t="s">
+        <v>280</v>
+      </c>
+      <c r="AO5" s="34" t="s">
+        <v>283</v>
+      </c>
+      <c r="AP5" s="34" t="s">
+        <v>286</v>
+      </c>
+      <c r="AQ5" s="34" t="s">
+        <v>254</v>
+      </c>
+      <c r="AR5" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="AS5" s="51" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="6" spans="1:45" s="29" customFormat="1" ht="70">
+      <c r="A6" s="52"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35" t="s">
+        <v>178</v>
+      </c>
+      <c r="G6" s="35" t="s">
+        <v>186</v>
+      </c>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="35"/>
+      <c r="K6" s="35" t="s">
+        <v>178</v>
+      </c>
+      <c r="L6" s="35" t="s">
+        <v>182</v>
+      </c>
+      <c r="M6" s="35" t="s">
+        <v>186</v>
+      </c>
+      <c r="N6" s="35">
+        <v>2</v>
+      </c>
+      <c r="O6" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="P6" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q6" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="R6" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="S6" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="T6" s="36" t="s">
+        <v>209</v>
+      </c>
+      <c r="U6" s="36" t="s">
+        <v>214</v>
+      </c>
+      <c r="V6" s="36" t="s">
+        <v>217</v>
+      </c>
+      <c r="W6" s="43" t="s">
+        <v>221</v>
+      </c>
+      <c r="X6" s="43" t="s">
+        <v>226</v>
+      </c>
+      <c r="Y6" s="36"/>
+      <c r="Z6" s="36" t="s">
+        <v>263</v>
+      </c>
+      <c r="AA6" s="43" t="s">
+        <v>230</v>
+      </c>
+      <c r="AB6" s="43" t="s">
+        <v>233</v>
+      </c>
+      <c r="AC6" s="43" t="s">
+        <v>230</v>
+      </c>
+      <c r="AD6" s="43" t="s">
+        <v>240</v>
+      </c>
+      <c r="AE6" s="43"/>
+      <c r="AF6" s="43"/>
+      <c r="AG6" s="43"/>
+      <c r="AH6" s="43"/>
+      <c r="AI6" s="43"/>
+      <c r="AJ6" s="43" t="s">
+        <v>267</v>
+      </c>
+      <c r="AK6" s="43"/>
+      <c r="AL6" s="43" t="s">
+        <v>277</v>
+      </c>
+      <c r="AM6" s="43"/>
+      <c r="AN6" s="43"/>
+      <c r="AO6" s="43"/>
+      <c r="AP6" s="43" t="s">
+        <v>287</v>
+      </c>
+      <c r="AQ6" s="43"/>
+      <c r="AR6" s="43"/>
+      <c r="AS6" s="53"/>
+    </row>
+    <row r="7" spans="1:45" s="29" customFormat="1">
+      <c r="A7" s="54" t="s">
+        <v>179</v>
+      </c>
+      <c r="B7" s="37" t="s">
+        <v>179</v>
+      </c>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="37"/>
+      <c r="J7" s="38" t="s">
         <v>185</v>
       </c>
-      <c r="F4" s="54" t="s">
-        <v>192</v>
-      </c>
-      <c r="G4" s="54" t="s">
-        <v>196</v>
-      </c>
-      <c r="H4" s="34" t="s">
-        <v>199</v>
-      </c>
-      <c r="I4" s="34" t="s">
-        <v>202</v>
-      </c>
-      <c r="J4" s="34" t="s">
-        <v>205</v>
-      </c>
-      <c r="K4" s="34" t="s">
-        <v>210</v>
-      </c>
-      <c r="L4" s="34" t="s">
-        <v>213</v>
-      </c>
-      <c r="M4" s="34" t="s">
-        <v>215</v>
-      </c>
-      <c r="N4" s="34" t="s">
-        <v>216</v>
-      </c>
-      <c r="O4" s="34" t="s">
-        <v>219</v>
-      </c>
-      <c r="P4" s="34" t="s">
-        <v>223</v>
-      </c>
-      <c r="Q4" s="34" t="s">
-        <v>226</v>
-      </c>
-      <c r="R4" s="34" t="s">
-        <v>230</v>
-      </c>
-      <c r="S4" s="34" t="s">
-        <v>234</v>
-      </c>
-      <c r="T4" s="34" t="s">
+      <c r="K7" s="37" t="s">
+        <v>179</v>
+      </c>
+      <c r="L7" s="37" t="s">
+        <v>179</v>
+      </c>
+      <c r="M7" s="38" t="s">
+        <v>185</v>
+      </c>
+      <c r="N7" s="37" t="s">
+        <v>179</v>
+      </c>
+      <c r="O7" s="37"/>
+      <c r="P7" s="37"/>
+      <c r="Q7" s="37"/>
+      <c r="R7" s="37"/>
+      <c r="S7" s="37"/>
+      <c r="T7" s="37" t="s">
+        <v>179</v>
+      </c>
+      <c r="U7" s="37" t="s">
+        <v>179</v>
+      </c>
+      <c r="V7" s="38" t="s">
+        <v>185</v>
+      </c>
+      <c r="W7" s="37"/>
+      <c r="X7" s="38"/>
+      <c r="Y7" s="37" t="s">
+        <v>179</v>
+      </c>
+      <c r="Z7" s="37"/>
+      <c r="AA7" s="37"/>
+      <c r="AB7" s="37"/>
+      <c r="AC7" s="37"/>
+      <c r="AD7" s="37"/>
+      <c r="AE7" s="37"/>
+      <c r="AF7" s="37"/>
+      <c r="AG7" s="37"/>
+      <c r="AH7" s="37"/>
+      <c r="AI7" s="37"/>
+      <c r="AJ7" s="37"/>
+      <c r="AK7" s="37"/>
+      <c r="AL7" s="37"/>
+      <c r="AM7" s="37"/>
+      <c r="AN7" s="37"/>
+      <c r="AO7" s="37"/>
+      <c r="AP7" s="37"/>
+      <c r="AQ7" s="37"/>
+      <c r="AR7" s="37"/>
+      <c r="AS7" s="55"/>
+    </row>
+    <row r="8" spans="1:45" s="29" customFormat="1" ht="15" thickBot="1">
+      <c r="A8" s="56" t="s">
+        <v>172</v>
+      </c>
+      <c r="B8" s="57" t="s">
+        <v>289</v>
+      </c>
+      <c r="C8" s="57" t="s">
+        <v>290</v>
+      </c>
+      <c r="D8" s="57" t="s">
+        <v>293</v>
+      </c>
+      <c r="E8" s="57" t="s">
+        <v>296</v>
+      </c>
+      <c r="F8" s="57" t="s">
+        <v>300</v>
+      </c>
+      <c r="G8" s="57" t="s">
+        <v>303</v>
+      </c>
+      <c r="H8" s="57" t="s">
+        <v>306</v>
+      </c>
+      <c r="I8" s="57" t="s">
+        <v>309</v>
+      </c>
+      <c r="J8" s="57" t="s">
+        <v>288</v>
+      </c>
+      <c r="K8" s="57" t="s">
+        <v>176</v>
+      </c>
+      <c r="L8" s="57" t="s">
+        <v>183</v>
+      </c>
+      <c r="M8" s="57" t="s">
+        <v>184</v>
+      </c>
+      <c r="N8" s="57" t="s">
+        <v>193</v>
+      </c>
+      <c r="O8" s="57" t="s">
+        <v>195</v>
+      </c>
+      <c r="P8" s="57" t="s">
+        <v>200</v>
+      </c>
+      <c r="Q8" s="57" t="s">
+        <v>201</v>
+      </c>
+      <c r="R8" s="58" t="s">
+        <v>203</v>
+      </c>
+      <c r="S8" s="58" t="s">
+        <v>206</v>
+      </c>
+      <c r="T8" s="58" t="s">
         <v>207</v>
       </c>
-      <c r="U4" s="34" t="s">
+      <c r="U8" s="58" t="s">
+        <v>211</v>
+      </c>
+      <c r="V8" s="58" t="s">
+        <v>218</v>
+      </c>
+      <c r="W8" s="58" t="s">
+        <v>222</v>
+      </c>
+      <c r="X8" s="58" t="s">
+        <v>224</v>
+      </c>
+      <c r="Y8" s="57" t="s">
+        <v>198</v>
+      </c>
+      <c r="Z8" s="57" t="s">
+        <v>260</v>
+      </c>
+      <c r="AA8" s="58" t="s">
+        <v>227</v>
+      </c>
+      <c r="AB8" s="58" t="s">
+        <v>232</v>
+      </c>
+      <c r="AC8" s="58" t="s">
+        <v>235</v>
+      </c>
+      <c r="AD8" s="58" t="s">
+        <v>238</v>
+      </c>
+      <c r="AE8" s="58" t="s">
+        <v>242</v>
+      </c>
+      <c r="AF8" s="58" t="s">
+        <v>244</v>
+      </c>
+      <c r="AG8" s="58" t="s">
+        <v>247</v>
+      </c>
+      <c r="AH8" s="58" t="s">
+        <v>249</v>
+      </c>
+      <c r="AI8" s="58" t="s">
+        <v>251</v>
+      </c>
+      <c r="AJ8" s="58" t="s">
+        <v>264</v>
+      </c>
+      <c r="AK8" s="58" t="s">
+        <v>270</v>
+      </c>
+      <c r="AL8" s="58" t="s">
+        <v>274</v>
+      </c>
+      <c r="AM8" s="58" t="s">
         <v>272</v>
       </c>
-      <c r="V4" s="34" t="s">
-        <v>239</v>
-      </c>
-      <c r="W4" s="34" t="s">
-        <v>242</v>
-      </c>
-      <c r="X4" s="34" t="s">
-        <v>245</v>
-      </c>
-      <c r="Y4" s="34" t="s">
-        <v>248</v>
-      </c>
-      <c r="Z4" s="34" t="s">
-        <v>252</v>
-      </c>
-      <c r="AA4" s="34" t="s">
-        <v>254</v>
-      </c>
-      <c r="AB4" s="34" t="s">
-        <v>257</v>
-      </c>
-      <c r="AC4" s="34" t="s">
-        <v>259</v>
-      </c>
-      <c r="AD4" s="34" t="s">
-        <v>261</v>
-      </c>
-      <c r="AE4" s="34" t="s">
-        <v>276</v>
-      </c>
-      <c r="AF4" s="34" t="s">
-        <v>279</v>
-      </c>
-      <c r="AG4" s="34" t="s">
-        <v>282</v>
-      </c>
-      <c r="AH4" s="34" t="s">
-        <v>286</v>
-      </c>
-      <c r="AI4" s="34" t="s">
-        <v>290</v>
-      </c>
-      <c r="AJ4" s="34" t="s">
-        <v>293</v>
-      </c>
-      <c r="AK4" s="34" t="s">
-        <v>296</v>
-      </c>
-      <c r="AL4" s="34" t="s">
-        <v>263</v>
-      </c>
-      <c r="AM4" s="53" t="s">
-        <v>266</v>
-      </c>
-      <c r="AN4" s="73" t="s">
-        <v>268</v>
-      </c>
-      <c r="AO4" s="45"/>
-    </row>
-    <row r="5" spans="1:41" s="38" customFormat="1" ht="154">
-      <c r="A5" s="64" t="s">
-        <v>175</v>
-      </c>
-      <c r="B5" s="55" t="s">
-        <v>178</v>
-      </c>
-      <c r="C5" s="55" t="s">
-        <v>195</v>
-      </c>
-      <c r="D5" s="55" t="s">
-        <v>182</v>
-      </c>
-      <c r="E5" s="56" t="s">
-        <v>186</v>
-      </c>
-      <c r="F5" s="56" t="s">
-        <v>193</v>
-      </c>
-      <c r="G5" s="53" t="s">
-        <v>197</v>
-      </c>
-      <c r="H5" s="47" t="s">
-        <v>200</v>
-      </c>
-      <c r="I5" s="47" t="s">
-        <v>203</v>
-      </c>
-      <c r="J5" s="47"/>
-      <c r="K5" s="47"/>
-      <c r="L5" s="47"/>
-      <c r="M5" s="47"/>
-      <c r="N5" s="47"/>
-      <c r="O5" s="47" t="s">
-        <v>221</v>
-      </c>
-      <c r="P5" s="47" t="s">
-        <v>224</v>
-      </c>
-      <c r="Q5" s="47" t="s">
-        <v>227</v>
-      </c>
-      <c r="R5" s="47" t="s">
-        <v>231</v>
-      </c>
-      <c r="S5" s="57" t="s">
-        <v>236</v>
-      </c>
-      <c r="T5" s="47" t="s">
-        <v>208</v>
-      </c>
-      <c r="U5" s="47" t="s">
-        <v>273</v>
-      </c>
-      <c r="V5" s="47" t="s">
-        <v>240</v>
-      </c>
-      <c r="W5" s="47" t="s">
-        <v>32</v>
-      </c>
-      <c r="X5" s="47" t="s">
-        <v>247</v>
-      </c>
-      <c r="Y5" s="47" t="s">
-        <v>250</v>
-      </c>
-      <c r="Z5" s="47" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA5" s="47" t="s">
+      <c r="AN8" s="58" t="s">
+        <v>278</v>
+      </c>
+      <c r="AO8" s="58" t="s">
+        <v>281</v>
+      </c>
+      <c r="AP8" s="58" t="s">
+        <v>284</v>
+      </c>
+      <c r="AQ8" s="58" t="s">
+        <v>253</v>
+      </c>
+      <c r="AR8" s="58" t="s">
         <v>256</v>
       </c>
-      <c r="AB5" s="47" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC5" s="47" t="s">
-        <v>52</v>
-      </c>
-      <c r="AD5" s="47" t="s">
-        <v>40</v>
-      </c>
-      <c r="AE5" s="47" t="s">
-        <v>277</v>
-      </c>
-      <c r="AF5" s="47" t="s">
-        <v>280</v>
-      </c>
-      <c r="AG5" s="47" t="s">
-        <v>284</v>
-      </c>
-      <c r="AH5" s="47" t="s">
-        <v>287</v>
-      </c>
-      <c r="AI5" s="47" t="s">
-        <v>291</v>
-      </c>
-      <c r="AJ5" s="47" t="s">
-        <v>294</v>
-      </c>
-      <c r="AK5" s="47" t="s">
-        <v>297</v>
-      </c>
-      <c r="AL5" s="47" t="s">
-        <v>265</v>
-      </c>
-      <c r="AM5" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="AN5" s="65" t="s">
-        <v>270</v>
-      </c>
-      <c r="AO5" s="32"/>
-    </row>
-    <row r="6" spans="1:41" s="40" customFormat="1" ht="70">
-      <c r="A6" s="66"/>
-      <c r="B6" s="48"/>
-      <c r="C6" s="48"/>
-      <c r="D6" s="48" t="s">
-        <v>183</v>
-      </c>
-      <c r="E6" s="48" t="s">
-        <v>187</v>
-      </c>
-      <c r="F6" s="48" t="s">
-        <v>191</v>
-      </c>
-      <c r="G6" s="48">
-        <v>2</v>
-      </c>
-      <c r="H6" s="48"/>
-      <c r="I6" s="48"/>
-      <c r="J6" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="K6" s="49" t="s">
-        <v>16</v>
-      </c>
-      <c r="L6" s="49" t="s">
-        <v>17</v>
-      </c>
-      <c r="M6" s="49" t="s">
-        <v>18</v>
-      </c>
-      <c r="N6" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="O6" s="49" t="s">
-        <v>220</v>
-      </c>
-      <c r="P6" s="49" t="s">
-        <v>225</v>
-      </c>
-      <c r="Q6" s="49" t="s">
-        <v>228</v>
-      </c>
-      <c r="R6" s="57" t="s">
-        <v>232</v>
-      </c>
-      <c r="S6" s="57" t="s">
-        <v>237</v>
-      </c>
-      <c r="T6" s="49"/>
-      <c r="U6" s="49" t="s">
-        <v>274</v>
-      </c>
-      <c r="V6" s="57" t="s">
-        <v>241</v>
-      </c>
-      <c r="W6" s="57" t="s">
-        <v>244</v>
-      </c>
-      <c r="X6" s="57" t="s">
-        <v>241</v>
-      </c>
-      <c r="Y6" s="57" t="s">
-        <v>251</v>
-      </c>
-      <c r="Z6" s="57"/>
-      <c r="AA6" s="57"/>
-      <c r="AB6" s="57"/>
-      <c r="AC6" s="57"/>
-      <c r="AD6" s="57"/>
-      <c r="AE6" s="57" t="s">
-        <v>278</v>
-      </c>
-      <c r="AF6" s="57"/>
-      <c r="AG6" s="57"/>
-      <c r="AH6" s="57" t="s">
-        <v>288</v>
-      </c>
-      <c r="AI6" s="57"/>
-      <c r="AJ6" s="57"/>
-      <c r="AK6" s="57" t="s">
-        <v>298</v>
-      </c>
-      <c r="AL6" s="57"/>
-      <c r="AM6" s="57"/>
-      <c r="AN6" s="67"/>
-      <c r="AO6" s="39"/>
-    </row>
-    <row r="7" spans="1:41" s="40" customFormat="1">
-      <c r="A7" s="68" t="s">
-        <v>184</v>
-      </c>
-      <c r="B7" s="50" t="s">
-        <v>184</v>
-      </c>
-      <c r="C7" s="51" t="s">
-        <v>190</v>
-      </c>
-      <c r="D7" s="50" t="s">
-        <v>184</v>
-      </c>
-      <c r="E7" s="50" t="s">
-        <v>184</v>
-      </c>
-      <c r="F7" s="51" t="s">
-        <v>190</v>
-      </c>
-      <c r="G7" s="50" t="s">
-        <v>184</v>
-      </c>
-      <c r="H7" s="50"/>
-      <c r="I7" s="50"/>
-      <c r="J7" s="50"/>
-      <c r="K7" s="50"/>
-      <c r="L7" s="50"/>
-      <c r="M7" s="50"/>
-      <c r="N7" s="50"/>
-      <c r="O7" s="50" t="s">
-        <v>184</v>
-      </c>
-      <c r="P7" s="50" t="s">
-        <v>184</v>
-      </c>
-      <c r="Q7" s="51" t="s">
-        <v>190</v>
-      </c>
-      <c r="R7" s="50"/>
-      <c r="S7" s="51"/>
-      <c r="T7" s="50" t="s">
-        <v>184</v>
-      </c>
-      <c r="U7" s="50"/>
-      <c r="V7" s="50"/>
-      <c r="W7" s="50"/>
-      <c r="X7" s="50"/>
-      <c r="Y7" s="50"/>
-      <c r="Z7" s="50"/>
-      <c r="AA7" s="50"/>
-      <c r="AB7" s="50"/>
-      <c r="AC7" s="50"/>
-      <c r="AD7" s="50"/>
-      <c r="AE7" s="50"/>
-      <c r="AF7" s="50"/>
-      <c r="AG7" s="50"/>
-      <c r="AH7" s="50"/>
-      <c r="AI7" s="50"/>
-      <c r="AJ7" s="50"/>
-      <c r="AK7" s="50"/>
-      <c r="AL7" s="50"/>
-      <c r="AM7" s="50"/>
-      <c r="AN7" s="69"/>
-      <c r="AO7" s="39"/>
-    </row>
-    <row r="8" spans="1:41" s="40" customFormat="1" ht="15" thickBot="1">
-      <c r="A8" s="70" t="s">
-        <v>176</v>
-      </c>
-      <c r="B8" s="71" t="s">
-        <v>179</v>
-      </c>
-      <c r="C8" s="71" t="s">
-        <v>299</v>
-      </c>
-      <c r="D8" s="71" t="s">
-        <v>181</v>
-      </c>
-      <c r="E8" s="71" t="s">
-        <v>188</v>
-      </c>
-      <c r="F8" s="71" t="s">
-        <v>189</v>
-      </c>
-      <c r="G8" s="71" t="s">
-        <v>198</v>
-      </c>
-      <c r="H8" s="71" t="s">
-        <v>201</v>
-      </c>
-      <c r="I8" s="71" t="s">
-        <v>204</v>
-      </c>
-      <c r="J8" s="71" t="s">
-        <v>206</v>
-      </c>
-      <c r="K8" s="71" t="s">
-        <v>211</v>
-      </c>
-      <c r="L8" s="71" t="s">
-        <v>212</v>
-      </c>
-      <c r="M8" s="72" t="s">
-        <v>214</v>
-      </c>
-      <c r="N8" s="72" t="s">
-        <v>217</v>
-      </c>
-      <c r="O8" s="72" t="s">
-        <v>218</v>
-      </c>
-      <c r="P8" s="72" t="s">
-        <v>222</v>
-      </c>
-      <c r="Q8" s="72" t="s">
-        <v>229</v>
-      </c>
-      <c r="R8" s="72" t="s">
-        <v>233</v>
-      </c>
-      <c r="S8" s="72" t="s">
-        <v>235</v>
-      </c>
-      <c r="T8" s="71" t="s">
-        <v>209</v>
-      </c>
-      <c r="U8" s="71" t="s">
-        <v>271</v>
-      </c>
-      <c r="V8" s="72" t="s">
-        <v>238</v>
-      </c>
-      <c r="W8" s="72" t="s">
-        <v>243</v>
-      </c>
-      <c r="X8" s="72" t="s">
-        <v>246</v>
-      </c>
-      <c r="Y8" s="72" t="s">
-        <v>249</v>
-      </c>
-      <c r="Z8" s="72" t="s">
-        <v>253</v>
-      </c>
-      <c r="AA8" s="72" t="s">
-        <v>255</v>
-      </c>
-      <c r="AB8" s="72" t="s">
+      <c r="AS8" s="59" t="s">
         <v>258</v>
       </c>
-      <c r="AC8" s="72" t="s">
-        <v>260</v>
-      </c>
-      <c r="AD8" s="72" t="s">
-        <v>262</v>
-      </c>
-      <c r="AE8" s="72" t="s">
-        <v>275</v>
-      </c>
-      <c r="AF8" s="72" t="s">
-        <v>281</v>
-      </c>
-      <c r="AG8" s="72" t="s">
-        <v>283</v>
-      </c>
-      <c r="AH8" s="72" t="s">
-        <v>285</v>
-      </c>
-      <c r="AI8" s="72" t="s">
-        <v>289</v>
-      </c>
-      <c r="AJ8" s="72" t="s">
-        <v>292</v>
-      </c>
-      <c r="AK8" s="72" t="s">
-        <v>295</v>
-      </c>
-      <c r="AL8" s="72" t="s">
-        <v>264</v>
-      </c>
-      <c r="AM8" s="72" t="s">
-        <v>267</v>
-      </c>
-      <c r="AN8" s="74" t="s">
-        <v>269</v>
-      </c>
-      <c r="AO8" s="39"/>
-    </row>
-    <row r="9" spans="1:41">
-      <c r="A9" s="75"/>
     </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4669,654 +5096,124 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:AN8"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C28" sqref="C28"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="39.5" style="8" customWidth="1"/>
-    <col min="2" max="25" width="39.5" style="11" customWidth="1"/>
-    <col min="26" max="40" width="39.5" customWidth="1"/>
+    <col min="2" max="2" width="39.5" style="11" customWidth="1"/>
+    <col min="3" max="6" width="39.5" style="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" ht="18">
-      <c r="A1" s="58" t="s">
-        <v>148</v>
-      </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59"/>
-      <c r="J1" s="59"/>
-      <c r="K1" s="59"/>
-      <c r="L1" s="59"/>
-      <c r="M1" s="59"/>
-      <c r="N1" s="59"/>
-      <c r="O1" s="59"/>
-      <c r="P1" s="59"/>
-      <c r="Q1" s="59"/>
-      <c r="R1" s="59"/>
-      <c r="S1" s="59"/>
-      <c r="T1" s="59"/>
-      <c r="U1" s="59"/>
-      <c r="V1" s="59"/>
-      <c r="W1" s="59"/>
-      <c r="X1" s="59"/>
-      <c r="Y1" s="59"/>
-      <c r="Z1" s="59"/>
-      <c r="AA1" s="59"/>
-      <c r="AB1" s="59"/>
-      <c r="AC1" s="59"/>
-      <c r="AD1" s="59"/>
-      <c r="AE1" s="59"/>
-      <c r="AF1" s="59"/>
-      <c r="AG1" s="59"/>
-      <c r="AH1" s="59"/>
-      <c r="AI1" s="59"/>
-      <c r="AJ1" s="59"/>
-      <c r="AK1" s="59"/>
-      <c r="AL1" s="59"/>
-      <c r="AM1" s="59"/>
-      <c r="AN1" s="60"/>
-    </row>
-    <row r="2" spans="1:40" ht="15">
-      <c r="A2" s="61" t="s">
-        <v>173</v>
-      </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="43"/>
-      <c r="L2" s="43"/>
-      <c r="M2" s="43"/>
-      <c r="N2" s="43"/>
-      <c r="O2" s="43"/>
-      <c r="P2" s="43"/>
-      <c r="Q2" s="43"/>
-      <c r="R2" s="43"/>
-      <c r="S2" s="43"/>
-      <c r="T2" s="43"/>
-      <c r="U2" s="43"/>
-      <c r="V2" s="43"/>
-      <c r="W2" s="43"/>
-      <c r="X2" s="43"/>
-      <c r="Y2" s="43"/>
-      <c r="Z2" s="43"/>
-      <c r="AA2" s="43"/>
-      <c r="AB2" s="43"/>
-      <c r="AC2" s="43"/>
-      <c r="AD2" s="43"/>
-      <c r="AE2" s="43"/>
-      <c r="AF2" s="43"/>
-      <c r="AG2" s="43"/>
-      <c r="AH2" s="43"/>
-      <c r="AI2" s="43"/>
-      <c r="AJ2" s="43"/>
-      <c r="AK2" s="43"/>
-      <c r="AL2" s="43"/>
-      <c r="AM2" s="43"/>
-      <c r="AN2" s="62"/>
-    </row>
-    <row r="3" spans="1:40" ht="15">
-      <c r="A3" s="61"/>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
-      <c r="K3" s="43"/>
-      <c r="L3" s="43"/>
-      <c r="M3" s="43"/>
-      <c r="N3" s="43"/>
-      <c r="O3" s="43"/>
-      <c r="P3" s="43"/>
-      <c r="Q3" s="43"/>
-      <c r="R3" s="43"/>
-      <c r="S3" s="43"/>
-      <c r="T3" s="43"/>
-      <c r="U3" s="43"/>
-      <c r="V3" s="43"/>
-      <c r="W3" s="43"/>
-      <c r="X3" s="43"/>
-      <c r="Y3" s="43"/>
-      <c r="Z3" s="43"/>
-      <c r="AA3" s="43"/>
-      <c r="AB3" s="43"/>
-      <c r="AC3" s="43"/>
-      <c r="AD3" s="43"/>
-      <c r="AE3" s="43"/>
-      <c r="AF3" s="43"/>
-      <c r="AG3" s="43"/>
-      <c r="AH3" s="43"/>
-      <c r="AI3" s="43"/>
-      <c r="AJ3" s="43"/>
-      <c r="AK3" s="43"/>
-      <c r="AL3" s="43"/>
-      <c r="AM3" s="43"/>
-      <c r="AN3" s="62"/>
-    </row>
-    <row r="4" spans="1:40">
-      <c r="A4" s="63" t="s">
-        <v>174</v>
-      </c>
-      <c r="B4" s="52" t="s">
-        <v>177</v>
-      </c>
-      <c r="C4" s="52" t="s">
-        <v>194</v>
-      </c>
-      <c r="D4" s="53" t="s">
-        <v>180</v>
-      </c>
-      <c r="E4" s="53" t="s">
-        <v>185</v>
-      </c>
-      <c r="F4" s="54" t="s">
-        <v>192</v>
-      </c>
-      <c r="G4" s="54" t="s">
-        <v>196</v>
-      </c>
-      <c r="H4" s="34" t="s">
-        <v>199</v>
-      </c>
-      <c r="I4" s="34" t="s">
-        <v>202</v>
-      </c>
-      <c r="J4" s="34" t="s">
-        <v>205</v>
-      </c>
-      <c r="K4" s="34" t="s">
-        <v>210</v>
-      </c>
-      <c r="L4" s="34" t="s">
-        <v>213</v>
-      </c>
-      <c r="M4" s="34" t="s">
-        <v>215</v>
-      </c>
-      <c r="N4" s="34" t="s">
-        <v>216</v>
-      </c>
-      <c r="O4" s="34" t="s">
-        <v>219</v>
-      </c>
-      <c r="P4" s="34" t="s">
-        <v>223</v>
-      </c>
-      <c r="Q4" s="34" t="s">
-        <v>226</v>
-      </c>
-      <c r="R4" s="34" t="s">
-        <v>230</v>
-      </c>
-      <c r="S4" s="34" t="s">
-        <v>234</v>
-      </c>
-      <c r="T4" s="34" t="s">
-        <v>207</v>
-      </c>
-      <c r="U4" s="34" t="s">
-        <v>272</v>
-      </c>
-      <c r="V4" s="34" t="s">
-        <v>239</v>
-      </c>
-      <c r="W4" s="34" t="s">
-        <v>242</v>
-      </c>
-      <c r="X4" s="34" t="s">
-        <v>245</v>
-      </c>
-      <c r="Y4" s="34" t="s">
-        <v>248</v>
-      </c>
-      <c r="Z4" s="34" t="s">
-        <v>252</v>
-      </c>
-      <c r="AA4" s="34" t="s">
-        <v>254</v>
-      </c>
-      <c r="AB4" s="34" t="s">
-        <v>257</v>
-      </c>
-      <c r="AC4" s="34" t="s">
-        <v>259</v>
-      </c>
-      <c r="AD4" s="34" t="s">
-        <v>261</v>
-      </c>
-      <c r="AE4" s="34" t="s">
-        <v>276</v>
-      </c>
-      <c r="AF4" s="34" t="s">
-        <v>279</v>
-      </c>
-      <c r="AG4" s="34" t="s">
-        <v>282</v>
-      </c>
-      <c r="AH4" s="34" t="s">
-        <v>286</v>
-      </c>
-      <c r="AI4" s="34" t="s">
-        <v>290</v>
-      </c>
-      <c r="AJ4" s="34" t="s">
-        <v>293</v>
-      </c>
-      <c r="AK4" s="34" t="s">
-        <v>296</v>
-      </c>
-      <c r="AL4" s="34" t="s">
-        <v>263</v>
-      </c>
-      <c r="AM4" s="53" t="s">
-        <v>266</v>
-      </c>
-      <c r="AN4" s="73" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="5" spans="1:40" ht="154">
-      <c r="A5" s="64" t="s">
-        <v>175</v>
-      </c>
-      <c r="B5" s="55" t="s">
-        <v>178</v>
-      </c>
-      <c r="C5" s="55" t="s">
-        <v>195</v>
-      </c>
-      <c r="D5" s="55" t="s">
-        <v>182</v>
-      </c>
-      <c r="E5" s="56" t="s">
-        <v>186</v>
-      </c>
-      <c r="F5" s="56" t="s">
-        <v>193</v>
-      </c>
-      <c r="G5" s="53" t="s">
-        <v>197</v>
-      </c>
-      <c r="H5" s="47" t="s">
-        <v>200</v>
-      </c>
-      <c r="I5" s="47" t="s">
-        <v>203</v>
-      </c>
-      <c r="J5" s="47"/>
-      <c r="K5" s="47"/>
-      <c r="L5" s="47"/>
-      <c r="M5" s="47"/>
-      <c r="N5" s="47"/>
-      <c r="O5" s="47" t="s">
-        <v>221</v>
-      </c>
-      <c r="P5" s="47" t="s">
-        <v>224</v>
-      </c>
-      <c r="Q5" s="47" t="s">
-        <v>227</v>
-      </c>
-      <c r="R5" s="47" t="s">
-        <v>231</v>
-      </c>
-      <c r="S5" s="57" t="s">
-        <v>236</v>
-      </c>
-      <c r="T5" s="47" t="s">
-        <v>208</v>
-      </c>
-      <c r="U5" s="47" t="s">
-        <v>273</v>
-      </c>
-      <c r="V5" s="47" t="s">
-        <v>240</v>
-      </c>
-      <c r="W5" s="47" t="s">
-        <v>32</v>
-      </c>
-      <c r="X5" s="47" t="s">
-        <v>247</v>
-      </c>
-      <c r="Y5" s="47" t="s">
-        <v>250</v>
-      </c>
-      <c r="Z5" s="47" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA5" s="47" t="s">
-        <v>256</v>
-      </c>
-      <c r="AB5" s="47" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC5" s="47" t="s">
-        <v>52</v>
-      </c>
-      <c r="AD5" s="47" t="s">
-        <v>40</v>
-      </c>
-      <c r="AE5" s="47" t="s">
-        <v>277</v>
-      </c>
-      <c r="AF5" s="47" t="s">
-        <v>280</v>
-      </c>
-      <c r="AG5" s="47" t="s">
-        <v>284</v>
-      </c>
-      <c r="AH5" s="47" t="s">
-        <v>287</v>
-      </c>
-      <c r="AI5" s="47" t="s">
-        <v>291</v>
-      </c>
-      <c r="AJ5" s="47" t="s">
-        <v>294</v>
-      </c>
-      <c r="AK5" s="47" t="s">
-        <v>297</v>
-      </c>
-      <c r="AL5" s="47" t="s">
-        <v>265</v>
-      </c>
-      <c r="AM5" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="AN5" s="65" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="6" spans="1:40" ht="70">
-      <c r="A6" s="66"/>
-      <c r="B6" s="48"/>
-      <c r="C6" s="48"/>
-      <c r="D6" s="48" t="s">
-        <v>183</v>
-      </c>
-      <c r="E6" s="48" t="s">
-        <v>187</v>
-      </c>
-      <c r="F6" s="48" t="s">
-        <v>191</v>
-      </c>
-      <c r="G6" s="48">
-        <v>2</v>
-      </c>
-      <c r="H6" s="48"/>
-      <c r="I6" s="48"/>
-      <c r="J6" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="K6" s="49" t="s">
-        <v>16</v>
-      </c>
-      <c r="L6" s="49" t="s">
-        <v>17</v>
-      </c>
-      <c r="M6" s="49" t="s">
-        <v>18</v>
-      </c>
-      <c r="N6" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="O6" s="49" t="s">
-        <v>220</v>
-      </c>
-      <c r="P6" s="49" t="s">
-        <v>225</v>
-      </c>
-      <c r="Q6" s="49" t="s">
-        <v>228</v>
-      </c>
-      <c r="R6" s="57" t="s">
-        <v>232</v>
-      </c>
-      <c r="S6" s="57" t="s">
-        <v>237</v>
-      </c>
-      <c r="T6" s="49"/>
-      <c r="U6" s="49" t="s">
-        <v>274</v>
-      </c>
-      <c r="V6" s="57" t="s">
-        <v>241</v>
-      </c>
-      <c r="W6" s="57" t="s">
-        <v>244</v>
-      </c>
-      <c r="X6" s="57" t="s">
-        <v>241</v>
-      </c>
-      <c r="Y6" s="57" t="s">
-        <v>251</v>
-      </c>
-      <c r="Z6" s="57"/>
-      <c r="AA6" s="57"/>
-      <c r="AB6" s="57"/>
-      <c r="AC6" s="57"/>
-      <c r="AD6" s="57"/>
-      <c r="AE6" s="57" t="s">
-        <v>278</v>
-      </c>
-      <c r="AF6" s="57"/>
-      <c r="AG6" s="57"/>
-      <c r="AH6" s="57" t="s">
-        <v>288</v>
-      </c>
-      <c r="AI6" s="57"/>
-      <c r="AJ6" s="57"/>
-      <c r="AK6" s="57" t="s">
-        <v>298</v>
-      </c>
-      <c r="AL6" s="57"/>
-      <c r="AM6" s="57"/>
-      <c r="AN6" s="67"/>
-    </row>
-    <row r="7" spans="1:40">
-      <c r="A7" s="68" t="s">
-        <v>184</v>
-      </c>
-      <c r="B7" s="50" t="s">
-        <v>184</v>
-      </c>
-      <c r="C7" s="51" t="s">
-        <v>190</v>
-      </c>
-      <c r="D7" s="50" t="s">
-        <v>184</v>
-      </c>
-      <c r="E7" s="50" t="s">
-        <v>184</v>
-      </c>
-      <c r="F7" s="51" t="s">
-        <v>190</v>
-      </c>
-      <c r="G7" s="50" t="s">
-        <v>184</v>
-      </c>
-      <c r="H7" s="50"/>
-      <c r="I7" s="50"/>
-      <c r="J7" s="50"/>
-      <c r="K7" s="50"/>
-      <c r="L7" s="50"/>
-      <c r="M7" s="50"/>
-      <c r="N7" s="50"/>
-      <c r="O7" s="50" t="s">
-        <v>184</v>
-      </c>
-      <c r="P7" s="50" t="s">
-        <v>184</v>
-      </c>
-      <c r="Q7" s="51" t="s">
-        <v>190</v>
-      </c>
-      <c r="R7" s="50"/>
-      <c r="S7" s="51"/>
-      <c r="T7" s="50" t="s">
-        <v>184</v>
-      </c>
-      <c r="U7" s="50"/>
-      <c r="V7" s="50"/>
-      <c r="W7" s="50"/>
-      <c r="X7" s="50"/>
-      <c r="Y7" s="50"/>
-      <c r="Z7" s="50"/>
-      <c r="AA7" s="50"/>
-      <c r="AB7" s="50"/>
-      <c r="AC7" s="50"/>
-      <c r="AD7" s="50"/>
-      <c r="AE7" s="50"/>
-      <c r="AF7" s="50"/>
-      <c r="AG7" s="50"/>
-      <c r="AH7" s="50"/>
-      <c r="AI7" s="50"/>
-      <c r="AJ7" s="50"/>
-      <c r="AK7" s="50"/>
-      <c r="AL7" s="50"/>
-      <c r="AM7" s="50"/>
-      <c r="AN7" s="69"/>
-    </row>
-    <row r="8" spans="1:40" ht="15" thickBot="1">
-      <c r="A8" s="70" t="s">
-        <v>176</v>
-      </c>
-      <c r="B8" s="71" t="s">
+    <row r="1" spans="1:6" ht="18">
+      <c r="A1" s="44" t="s">
+        <v>327</v>
+      </c>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="46"/>
+    </row>
+    <row r="2" spans="1:6" ht="15">
+      <c r="A2" s="47" t="s">
+        <v>328</v>
+      </c>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="48"/>
+    </row>
+    <row r="3" spans="1:6" ht="15">
+      <c r="A3" s="47"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="48"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="49" t="s">
+        <v>170</v>
+      </c>
+      <c r="B4" s="65" t="s">
+        <v>312</v>
+      </c>
+      <c r="C4" s="65" t="s">
+        <v>315</v>
+      </c>
+      <c r="D4" s="65" t="s">
+        <v>318</v>
+      </c>
+      <c r="E4" s="65" t="s">
+        <v>321</v>
+      </c>
+      <c r="F4" s="61" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="70">
+      <c r="A5" s="50" t="s">
+        <v>311</v>
+      </c>
+      <c r="B5" s="41" t="s">
+        <v>314</v>
+      </c>
+      <c r="C5" s="41" t="s">
+        <v>317</v>
+      </c>
+      <c r="D5" s="41" t="s">
+        <v>320</v>
+      </c>
+      <c r="E5" s="41" t="s">
+        <v>323</v>
+      </c>
+      <c r="F5" s="62" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="52"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="63"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="54" t="s">
         <v>179</v>
       </c>
-      <c r="C8" s="71" t="s">
-        <v>299</v>
-      </c>
-      <c r="D8" s="71" t="s">
-        <v>181</v>
-      </c>
-      <c r="E8" s="71" t="s">
-        <v>188</v>
-      </c>
-      <c r="F8" s="71" t="s">
-        <v>189</v>
-      </c>
-      <c r="G8" s="71" t="s">
-        <v>198</v>
-      </c>
-      <c r="H8" s="71" t="s">
-        <v>201</v>
-      </c>
-      <c r="I8" s="71" t="s">
-        <v>204</v>
-      </c>
-      <c r="J8" s="71" t="s">
-        <v>206</v>
-      </c>
-      <c r="K8" s="71" t="s">
-        <v>211</v>
-      </c>
-      <c r="L8" s="71" t="s">
-        <v>212</v>
-      </c>
-      <c r="M8" s="72" t="s">
-        <v>214</v>
-      </c>
-      <c r="N8" s="72" t="s">
-        <v>217</v>
-      </c>
-      <c r="O8" s="72" t="s">
-        <v>218</v>
-      </c>
-      <c r="P8" s="72" t="s">
-        <v>222</v>
-      </c>
-      <c r="Q8" s="72" t="s">
-        <v>229</v>
-      </c>
-      <c r="R8" s="72" t="s">
-        <v>233</v>
-      </c>
-      <c r="S8" s="72" t="s">
-        <v>235</v>
-      </c>
-      <c r="T8" s="71" t="s">
-        <v>209</v>
-      </c>
-      <c r="U8" s="71" t="s">
-        <v>271</v>
-      </c>
-      <c r="V8" s="72" t="s">
-        <v>238</v>
-      </c>
-      <c r="W8" s="72" t="s">
-        <v>243</v>
-      </c>
-      <c r="X8" s="72" t="s">
-        <v>246</v>
-      </c>
-      <c r="Y8" s="72" t="s">
-        <v>249</v>
-      </c>
-      <c r="Z8" s="72" t="s">
-        <v>253</v>
-      </c>
-      <c r="AA8" s="72" t="s">
-        <v>255</v>
-      </c>
-      <c r="AB8" s="72" t="s">
-        <v>258</v>
-      </c>
-      <c r="AC8" s="72" t="s">
-        <v>260</v>
-      </c>
-      <c r="AD8" s="72" t="s">
-        <v>262</v>
-      </c>
-      <c r="AE8" s="72" t="s">
-        <v>275</v>
-      </c>
-      <c r="AF8" s="72" t="s">
-        <v>281</v>
-      </c>
-      <c r="AG8" s="72" t="s">
-        <v>283</v>
-      </c>
-      <c r="AH8" s="72" t="s">
-        <v>285</v>
-      </c>
-      <c r="AI8" s="72" t="s">
-        <v>289</v>
-      </c>
-      <c r="AJ8" s="72" t="s">
-        <v>292</v>
-      </c>
-      <c r="AK8" s="72" t="s">
-        <v>295</v>
-      </c>
-      <c r="AL8" s="72" t="s">
-        <v>264</v>
-      </c>
-      <c r="AM8" s="72" t="s">
-        <v>267</v>
-      </c>
-      <c r="AN8" s="74" t="s">
-        <v>269</v>
+      <c r="B7" s="37"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="55"/>
+    </row>
+    <row r="8" spans="1:6" ht="15" thickBot="1">
+      <c r="A8" s="56" t="s">
+        <v>172</v>
+      </c>
+      <c r="B8" s="57" t="s">
+        <v>313</v>
+      </c>
+      <c r="C8" s="57" t="s">
+        <v>316</v>
+      </c>
+      <c r="D8" s="57" t="s">
+        <v>319</v>
+      </c>
+      <c r="E8" s="57" t="s">
+        <v>322</v>
+      </c>
+      <c r="F8" s="64" t="s">
+        <v>325</v>
       </c>
     </row>
   </sheetData>
@@ -5333,197 +5230,338 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:AU9"/>
+  <dimension ref="A1:T8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="28.6640625" style="8" customWidth="1"/>
-    <col min="2" max="2" width="26.33203125" style="11" customWidth="1"/>
-    <col min="3" max="3" width="29.33203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.33203125" style="11" customWidth="1"/>
-    <col min="5" max="5" width="22.83203125" style="11" customWidth="1"/>
-    <col min="6" max="7" width="24.33203125" style="11" customWidth="1"/>
-    <col min="8" max="8" width="40" style="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="33.5" style="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.5" style="11" customWidth="1"/>
-    <col min="11" max="11" width="28.5" style="11" customWidth="1"/>
-    <col min="12" max="17" width="41.1640625" style="11" customWidth="1"/>
-    <col min="18" max="47" width="8.83203125" style="11"/>
+    <col min="1" max="1" width="39.5" style="8" customWidth="1"/>
+    <col min="2" max="20" width="39.5" style="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" ht="15" customHeight="1">
-      <c r="A1" s="11" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="2" spans="1:47" s="21" customFormat="1" ht="45" customHeight="1">
-      <c r="A2" s="23" t="s">
-        <v>157</v>
-      </c>
-      <c r="B2" s="22" t="s">
-        <v>131</v>
-      </c>
-      <c r="C2" s="22" t="s">
-        <v>132</v>
-      </c>
-      <c r="D2" s="22" t="s">
-        <v>133</v>
-      </c>
-      <c r="E2" s="22" t="s">
-        <v>134</v>
-      </c>
-      <c r="F2" s="22" t="s">
-        <v>135</v>
-      </c>
-      <c r="G2" s="22" t="s">
-        <v>135</v>
-      </c>
-      <c r="H2" s="22" t="s">
-        <v>136</v>
-      </c>
-      <c r="I2" s="22" t="s">
-        <v>137</v>
-      </c>
-      <c r="J2" s="22" t="s">
-        <v>138</v>
-      </c>
-      <c r="K2" s="22" t="s">
-        <v>139</v>
-      </c>
-      <c r="L2" s="22" t="s">
-        <v>140</v>
-      </c>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
-      <c r="P2" s="20"/>
-      <c r="Q2" s="20"/>
-      <c r="R2" s="20"/>
-      <c r="S2" s="20"/>
-      <c r="T2" s="20"/>
-      <c r="U2" s="20"/>
-      <c r="V2" s="20"/>
-      <c r="W2" s="20"/>
-      <c r="X2" s="20"/>
-      <c r="Y2" s="20"/>
-      <c r="Z2" s="20"/>
-      <c r="AA2" s="20"/>
-      <c r="AB2" s="20"/>
-      <c r="AC2" s="20"/>
-      <c r="AD2" s="20"/>
-      <c r="AE2" s="20"/>
-      <c r="AF2" s="20"/>
-      <c r="AG2" s="20"/>
-      <c r="AH2" s="20"/>
-      <c r="AI2" s="20"/>
-      <c r="AJ2" s="20"/>
-      <c r="AK2" s="20"/>
-      <c r="AL2" s="20"/>
-      <c r="AM2" s="20"/>
-      <c r="AN2" s="20"/>
-      <c r="AO2" s="20"/>
-      <c r="AP2" s="20"/>
-      <c r="AQ2" s="20"/>
-      <c r="AR2" s="20"/>
-      <c r="AS2" s="20"/>
-      <c r="AT2" s="20"/>
-      <c r="AU2" s="20"/>
-    </row>
-    <row r="3" spans="1:47" s="19" customFormat="1" ht="105" customHeight="1">
-      <c r="A3" s="24" t="s">
-        <v>159</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>143</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="K3" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="M3" s="17"/>
-      <c r="N3" s="17"/>
-      <c r="O3" s="17"/>
-      <c r="P3" s="17"/>
-      <c r="Q3" s="17"/>
-      <c r="R3" s="17"/>
-      <c r="S3" s="17"/>
-      <c r="T3" s="17"/>
-      <c r="U3" s="17"/>
-      <c r="V3" s="17"/>
-      <c r="W3" s="17"/>
-      <c r="X3" s="17"/>
-      <c r="Y3" s="17"/>
-      <c r="Z3" s="17"/>
-      <c r="AA3" s="17"/>
-      <c r="AB3" s="17"/>
-      <c r="AC3" s="17"/>
-      <c r="AD3" s="17"/>
-      <c r="AE3" s="17"/>
-      <c r="AF3" s="17"/>
-      <c r="AG3" s="17"/>
-      <c r="AH3" s="17"/>
-      <c r="AI3" s="17"/>
-      <c r="AJ3" s="17"/>
-      <c r="AK3" s="17"/>
-      <c r="AL3" s="17"/>
-      <c r="AM3" s="17"/>
-      <c r="AN3" s="17"/>
-      <c r="AO3" s="17"/>
-      <c r="AP3" s="17"/>
-      <c r="AQ3" s="17"/>
-      <c r="AR3" s="17"/>
-      <c r="AS3" s="17"/>
-      <c r="AT3" s="17"/>
-      <c r="AU3" s="17"/>
-    </row>
-    <row r="4" spans="1:47">
-      <c r="D4" s="7"/>
-    </row>
-    <row r="5" spans="1:47">
-      <c r="D5" s="7"/>
-    </row>
-    <row r="6" spans="1:47">
-      <c r="D6" s="7"/>
-    </row>
-    <row r="7" spans="1:47">
-      <c r="D7" s="7"/>
-    </row>
-    <row r="8" spans="1:47">
-      <c r="D8" s="7"/>
-    </row>
-    <row r="9" spans="1:47">
-      <c r="D9" s="7"/>
+    <row r="1" spans="1:20" ht="18">
+      <c r="A1" s="44" t="s">
+        <v>329</v>
+      </c>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
+      <c r="N1" s="45"/>
+      <c r="O1" s="45"/>
+      <c r="P1" s="45"/>
+      <c r="Q1" s="45"/>
+      <c r="R1" s="45"/>
+      <c r="S1" s="45"/>
+      <c r="T1" s="46"/>
+    </row>
+    <row r="2" spans="1:20" s="18" customFormat="1" ht="15">
+      <c r="A2" s="47" t="s">
+        <v>330</v>
+      </c>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="31"/>
+      <c r="P2" s="31"/>
+      <c r="Q2" s="31"/>
+      <c r="R2" s="31"/>
+      <c r="S2" s="31"/>
+      <c r="T2" s="48"/>
+    </row>
+    <row r="3" spans="1:20" s="18" customFormat="1" ht="15">
+      <c r="A3" s="47"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="31"/>
+      <c r="N3" s="31"/>
+      <c r="O3" s="31"/>
+      <c r="P3" s="31"/>
+      <c r="Q3" s="31"/>
+      <c r="R3" s="31"/>
+      <c r="S3" s="31"/>
+      <c r="T3" s="48"/>
+    </row>
+    <row r="4" spans="1:20" s="69" customFormat="1">
+      <c r="A4" s="49" t="s">
+        <v>170</v>
+      </c>
+      <c r="B4" s="65" t="s">
+        <v>332</v>
+      </c>
+      <c r="C4" s="65" t="s">
+        <v>336</v>
+      </c>
+      <c r="D4" s="65" t="s">
+        <v>338</v>
+      </c>
+      <c r="E4" s="39" t="s">
+        <v>341</v>
+      </c>
+      <c r="F4" s="39" t="s">
+        <v>344</v>
+      </c>
+      <c r="G4" s="65" t="s">
+        <v>346</v>
+      </c>
+      <c r="H4" s="65" t="s">
+        <v>351</v>
+      </c>
+      <c r="I4" s="65" t="s">
+        <v>393</v>
+      </c>
+      <c r="J4" s="65" t="s">
+        <v>358</v>
+      </c>
+      <c r="K4" s="65" t="s">
+        <v>361</v>
+      </c>
+      <c r="L4" s="65" t="s">
+        <v>364</v>
+      </c>
+      <c r="M4" s="67" t="s">
+        <v>367</v>
+      </c>
+      <c r="N4" s="67" t="s">
+        <v>371</v>
+      </c>
+      <c r="O4" s="65" t="s">
+        <v>374</v>
+      </c>
+      <c r="P4" s="65" t="s">
+        <v>377</v>
+      </c>
+      <c r="Q4" s="65" t="s">
+        <v>380</v>
+      </c>
+      <c r="R4" s="65" t="s">
+        <v>383</v>
+      </c>
+      <c r="S4" s="65" t="s">
+        <v>386</v>
+      </c>
+      <c r="T4" s="70" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" s="18" customFormat="1" ht="224">
+      <c r="A5" s="50" t="s">
+        <v>331</v>
+      </c>
+      <c r="B5" s="41" t="s">
+        <v>334</v>
+      </c>
+      <c r="C5" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="41" t="s">
+        <v>339</v>
+      </c>
+      <c r="E5" s="41" t="s">
+        <v>342</v>
+      </c>
+      <c r="F5" s="41" t="s">
+        <v>345</v>
+      </c>
+      <c r="G5" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="H5" s="41" t="s">
+        <v>353</v>
+      </c>
+      <c r="I5" s="41" t="s">
+        <v>356</v>
+      </c>
+      <c r="J5" s="41" t="s">
+        <v>360</v>
+      </c>
+      <c r="K5" s="41" t="s">
+        <v>363</v>
+      </c>
+      <c r="L5" s="42" t="s">
+        <v>366</v>
+      </c>
+      <c r="M5" s="42" t="s">
+        <v>368</v>
+      </c>
+      <c r="N5" s="34" t="s">
+        <v>372</v>
+      </c>
+      <c r="O5" s="34" t="s">
+        <v>375</v>
+      </c>
+      <c r="P5" s="34" t="s">
+        <v>379</v>
+      </c>
+      <c r="Q5" s="34" t="s">
+        <v>382</v>
+      </c>
+      <c r="R5" s="34" t="s">
+        <v>385</v>
+      </c>
+      <c r="S5" s="34" t="s">
+        <v>387</v>
+      </c>
+      <c r="T5" s="51" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" s="18" customFormat="1" ht="28">
+      <c r="A6" s="52"/>
+      <c r="B6" s="35" t="s">
+        <v>335</v>
+      </c>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35" t="s">
+        <v>340</v>
+      </c>
+      <c r="E6" s="35" t="s">
+        <v>343</v>
+      </c>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35" t="s">
+        <v>186</v>
+      </c>
+      <c r="H6" s="35" t="s">
+        <v>354</v>
+      </c>
+      <c r="I6" s="35" t="s">
+        <v>357</v>
+      </c>
+      <c r="J6" s="35"/>
+      <c r="K6" s="35"/>
+      <c r="L6" s="35"/>
+      <c r="M6" s="35" t="s">
+        <v>369</v>
+      </c>
+      <c r="N6" s="35"/>
+      <c r="O6" s="36"/>
+      <c r="P6" s="36"/>
+      <c r="Q6" s="36"/>
+      <c r="R6" s="36"/>
+      <c r="S6" s="36" t="s">
+        <v>392</v>
+      </c>
+      <c r="T6" s="71"/>
+    </row>
+    <row r="7" spans="1:20" s="18" customFormat="1">
+      <c r="A7" s="54" t="s">
+        <v>179</v>
+      </c>
+      <c r="B7" s="37"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="37"/>
+      <c r="J7" s="38"/>
+      <c r="K7" s="37"/>
+      <c r="L7" s="37"/>
+      <c r="M7" s="38"/>
+      <c r="N7" s="37"/>
+      <c r="O7" s="37"/>
+      <c r="P7" s="37"/>
+      <c r="Q7" s="37"/>
+      <c r="R7" s="37"/>
+      <c r="S7" s="37" t="s">
+        <v>179</v>
+      </c>
+      <c r="T7" s="55"/>
+    </row>
+    <row r="8" spans="1:20" s="17" customFormat="1" ht="15" thickBot="1">
+      <c r="A8" s="56" t="s">
+        <v>172</v>
+      </c>
+      <c r="B8" s="57" t="s">
+        <v>333</v>
+      </c>
+      <c r="C8" s="57" t="s">
+        <v>337</v>
+      </c>
+      <c r="D8" s="57" t="s">
+        <v>347</v>
+      </c>
+      <c r="E8" s="57" t="s">
+        <v>348</v>
+      </c>
+      <c r="F8" s="57" t="s">
+        <v>349</v>
+      </c>
+      <c r="G8" s="57" t="s">
+        <v>350</v>
+      </c>
+      <c r="H8" s="57" t="s">
+        <v>352</v>
+      </c>
+      <c r="I8" s="57" t="s">
+        <v>355</v>
+      </c>
+      <c r="J8" s="57" t="s">
+        <v>359</v>
+      </c>
+      <c r="K8" s="57" t="s">
+        <v>362</v>
+      </c>
+      <c r="L8" s="57" t="s">
+        <v>365</v>
+      </c>
+      <c r="M8" s="57" t="s">
+        <v>370</v>
+      </c>
+      <c r="N8" s="57" t="s">
+        <v>373</v>
+      </c>
+      <c r="O8" s="57" t="s">
+        <v>376</v>
+      </c>
+      <c r="P8" s="57" t="s">
+        <v>378</v>
+      </c>
+      <c r="Q8" s="57" t="s">
+        <v>381</v>
+      </c>
+      <c r="R8" s="58" t="s">
+        <v>384</v>
+      </c>
+      <c r="S8" s="58" t="s">
+        <v>388</v>
+      </c>
+      <c r="T8" s="59" t="s">
+        <v>390</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5558,7 +5596,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B1" s="15" t="s">
         <v>6</v>
@@ -5574,20 +5612,20 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="56">
-      <c r="A2" s="33"/>
-      <c r="B2" s="25" t="s">
-        <v>147</v>
-      </c>
-      <c r="C2" s="26" t="s">
-        <v>159</v>
-      </c>
-      <c r="D2" s="24" t="s">
-        <v>161</v>
+      <c r="A2" s="60"/>
+      <c r="B2" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>156</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>157</v>
       </c>
       <c r="E2" s="5"/>
     </row>
     <row r="3" spans="1:5" ht="42">
-      <c r="A3" s="33"/>
+      <c r="A3" s="60"/>
       <c r="B3" s="5" t="s">
         <v>11</v>
       </c>
@@ -5602,9 +5640,9 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="140">
-      <c r="A4" s="33"/>
+      <c r="A4" s="60"/>
       <c r="B4" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>12</v>
@@ -5617,9 +5655,9 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="70">
-      <c r="A5" s="33"/>
+      <c r="A5" s="60"/>
       <c r="B5" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>54</v>
@@ -5632,9 +5670,9 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="98">
-      <c r="A6" s="33"/>
+      <c r="A6" s="60"/>
       <c r="B6" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>55</v>
@@ -5645,9 +5683,9 @@
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:5" ht="42">
-      <c r="A7" s="33"/>
+      <c r="A7" s="60"/>
       <c r="B7" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>57</v>
@@ -5658,9 +5696,9 @@
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5" ht="28">
-      <c r="A8" s="33"/>
+      <c r="A8" s="60"/>
       <c r="B8" s="5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>59</v>
@@ -5671,9 +5709,9 @@
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:5" ht="56">
-      <c r="A9" s="33"/>
+      <c r="A9" s="60"/>
       <c r="B9" s="16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>58</v>
@@ -5684,9 +5722,9 @@
       <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="33"/>
+      <c r="A10" s="60"/>
       <c r="B10" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>60</v>
@@ -5697,9 +5735,9 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="28">
-      <c r="A11" s="33"/>
+      <c r="A11" s="60"/>
       <c r="B11" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>61</v>
@@ -5710,9 +5748,9 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="28">
-      <c r="A12" s="33"/>
+      <c r="A12" s="60"/>
       <c r="B12" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>62</v>
@@ -5723,9 +5761,9 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="28">
-      <c r="A13" s="33"/>
+      <c r="A13" s="60"/>
       <c r="B13" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>63</v>
@@ -5736,9 +5774,9 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="28">
-      <c r="A14" s="33"/>
+      <c r="A14" s="60"/>
       <c r="B14" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>64</v>
@@ -5749,9 +5787,9 @@
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="33"/>
+      <c r="A15" s="60"/>
       <c r="B15" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>65</v>
@@ -5764,9 +5802,9 @@
       </c>
     </row>
     <row r="16" spans="1:5" ht="28">
-      <c r="A16" s="33"/>
+      <c r="A16" s="60"/>
       <c r="B16" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>66</v>
@@ -5779,9 +5817,9 @@
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="33"/>
+      <c r="A17" s="60"/>
       <c r="B17" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>67</v>
@@ -5794,24 +5832,24 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="56">
-      <c r="A18" s="33"/>
+      <c r="A18" s="60"/>
       <c r="B18" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>68</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="33"/>
+      <c r="A19" s="60"/>
       <c r="B19" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>69</v>
@@ -5824,9 +5862,9 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="28">
-      <c r="A20" s="33"/>
+      <c r="A20" s="60"/>
       <c r="B20" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>70</v>
@@ -5839,9 +5877,9 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="70">
-      <c r="A21" s="33"/>
+      <c r="A21" s="60"/>
       <c r="B21" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>71</v>
@@ -5852,9 +5890,9 @@
       <c r="E21" s="1"/>
     </row>
     <row r="22" spans="1:7" ht="42">
-      <c r="A22" s="33"/>
+      <c r="A22" s="60"/>
       <c r="B22" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>72</v>
@@ -5867,9 +5905,9 @@
       </c>
     </row>
     <row r="23" spans="1:7" ht="28">
-      <c r="A23" s="33"/>
+      <c r="A23" s="60"/>
       <c r="B23" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>73</v>
@@ -5880,26 +5918,26 @@
       <c r="E23" s="1"/>
     </row>
     <row r="24" spans="1:7" ht="120" customHeight="1">
-      <c r="A24" s="33"/>
-      <c r="B24" s="27" t="s">
-        <v>153</v>
+      <c r="A24" s="60"/>
+      <c r="B24" s="22" t="s">
+        <v>151</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="E24" s="31" t="s">
-        <v>169</v>
-      </c>
-      <c r="F24" s="30"/>
-      <c r="G24" s="30"/>
+        <v>149</v>
+      </c>
+      <c r="E24" s="26" t="s">
+        <v>165</v>
+      </c>
+      <c r="F24" s="25"/>
+      <c r="G24" s="25"/>
     </row>
     <row r="25" spans="1:7" ht="36">
-      <c r="A25" s="33"/>
+      <c r="A25" s="60"/>
       <c r="B25" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C25" s="14" t="s">
         <v>74</v>
@@ -5907,16 +5945,16 @@
       <c r="D25" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E25" s="30"/>
-      <c r="F25" s="30"/>
-      <c r="G25" s="31" t="s">
-        <v>170</v>
+      <c r="E25" s="25"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="26" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="60">
-      <c r="A26" s="33"/>
+      <c r="A26" s="60"/>
       <c r="B26" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C26" s="14" t="s">
         <v>75</v>
@@ -5924,14 +5962,14 @@
       <c r="D26" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E26" s="28" t="s">
-        <v>154</v>
+      <c r="E26" s="23" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="28">
-      <c r="A27" s="33"/>
+      <c r="A27" s="60"/>
       <c r="B27" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>76</v>
@@ -5942,12 +5980,12 @@
       <c r="E27" s="1"/>
     </row>
     <row r="28" spans="1:7" ht="56">
-      <c r="A28" s="33"/>
+      <c r="A28" s="60"/>
       <c r="B28" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>38</v>
@@ -5955,12 +5993,12 @@
       <c r="E28" s="1"/>
     </row>
     <row r="29" spans="1:7" ht="28">
-      <c r="A29" s="33"/>
+      <c r="A29" s="60"/>
       <c r="B29" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>39</v>
@@ -5968,12 +6006,12 @@
       <c r="E29" s="1"/>
     </row>
     <row r="30" spans="1:7" ht="112">
-      <c r="A30" s="33"/>
+      <c r="A30" s="60"/>
       <c r="B30" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>52</v>
@@ -5981,9 +6019,9 @@
       <c r="E30" s="1"/>
     </row>
     <row r="31" spans="1:7" ht="28">
-      <c r="A31" s="33"/>
+      <c r="A31" s="60"/>
       <c r="B31" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C31" s="6" t="s">
         <v>77</v>
@@ -5995,10 +6033,10 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>78</v>
@@ -6007,22 +6045,22 @@
       <c r="E32" s="1"/>
     </row>
     <row r="33" spans="1:5" ht="56">
-      <c r="A33" s="33"/>
-      <c r="B33" s="25" t="s">
-        <v>147</v>
-      </c>
-      <c r="C33" s="26" t="s">
-        <v>146</v>
-      </c>
-      <c r="D33" s="24" t="s">
-        <v>162</v>
+      <c r="A33" s="60"/>
+      <c r="B33" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="C33" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="D33" s="19" t="s">
+        <v>158</v>
       </c>
       <c r="E33" s="5"/>
     </row>
     <row r="34" spans="1:5" ht="28">
-      <c r="A34" s="33"/>
+      <c r="A34" s="60"/>
       <c r="B34" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>79</v>
@@ -6033,25 +6071,25 @@
       <c r="E34" s="1"/>
     </row>
     <row r="35" spans="1:5" ht="28">
-      <c r="A35" s="33"/>
+      <c r="A35" s="60"/>
       <c r="B35" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E35" s="1"/>
     </row>
     <row r="36" spans="1:5" ht="56">
-      <c r="A36" s="33"/>
+      <c r="A36" s="60"/>
       <c r="B36" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>42</v>
@@ -6059,9 +6097,9 @@
       <c r="E36" s="1"/>
     </row>
     <row r="37" spans="1:5" ht="28">
-      <c r="A37" s="33"/>
+      <c r="A37" s="60"/>
       <c r="B37" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>80</v>
@@ -6072,11 +6110,11 @@
       <c r="E37" s="1"/>
     </row>
     <row r="38" spans="1:5" ht="28">
-      <c r="A38" s="29" t="s">
-        <v>166</v>
+      <c r="A38" s="24" t="s">
+        <v>162</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>81</v>
@@ -6085,22 +6123,22 @@
       <c r="E38" s="1"/>
     </row>
     <row r="39" spans="1:5" ht="56">
-      <c r="A39" s="33"/>
-      <c r="B39" s="25" t="s">
-        <v>147</v>
-      </c>
-      <c r="C39" s="26" t="s">
-        <v>146</v>
-      </c>
-      <c r="D39" s="24" t="s">
-        <v>163</v>
+      <c r="A39" s="60"/>
+      <c r="B39" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="C39" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="D39" s="19" t="s">
+        <v>159</v>
       </c>
       <c r="E39" s="5"/>
     </row>
     <row r="40" spans="1:5">
-      <c r="A40" s="33"/>
+      <c r="A40" s="60"/>
       <c r="B40" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C40" s="6" t="s">
         <v>82</v>
@@ -6113,9 +6151,9 @@
       </c>
     </row>
     <row r="41" spans="1:5" ht="42">
-      <c r="A41" s="33"/>
+      <c r="A41" s="60"/>
       <c r="B41" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C41" s="6" t="s">
         <v>83</v>
@@ -6126,9 +6164,9 @@
       <c r="E41" s="1"/>
     </row>
     <row r="42" spans="1:5" ht="84">
-      <c r="A42" s="33"/>
+      <c r="A42" s="60"/>
       <c r="B42" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>85</v>
@@ -6139,9 +6177,9 @@
       <c r="E42" s="7"/>
     </row>
     <row r="43" spans="1:5" ht="56">
-      <c r="A43" s="33"/>
+      <c r="A43" s="60"/>
       <c r="B43" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C43" s="6" t="s">
         <v>87</v>
@@ -6152,9 +6190,9 @@
       <c r="E43" s="1"/>
     </row>
     <row r="44" spans="1:5" ht="56">
-      <c r="A44" s="33"/>
+      <c r="A44" s="60"/>
       <c r="B44" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C44" s="6" t="s">
         <v>88</v>
@@ -6165,9 +6203,9 @@
       <c r="E44" s="1"/>
     </row>
     <row r="45" spans="1:5" ht="56">
-      <c r="A45" s="33"/>
+      <c r="A45" s="60"/>
       <c r="B45" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C45" s="6" t="s">
         <v>88</v>
@@ -6178,9 +6216,9 @@
       <c r="E45" s="1"/>
     </row>
     <row r="46" spans="1:5" ht="29">
-      <c r="A46" s="33"/>
+      <c r="A46" s="60"/>
       <c r="B46" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C46" s="6" t="s">
         <v>89</v>
@@ -6191,9 +6229,9 @@
       <c r="E46" s="1"/>
     </row>
     <row r="47" spans="1:5" ht="42">
-      <c r="A47" s="33"/>
+      <c r="A47" s="60"/>
       <c r="B47" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C47" s="6" t="s">
         <v>90</v>
@@ -6204,9 +6242,9 @@
       <c r="E47" s="1"/>
     </row>
     <row r="48" spans="1:5" ht="406">
-      <c r="A48" s="33"/>
+      <c r="A48" s="60"/>
       <c r="B48" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C48" s="6" t="s">
         <v>91</v>
@@ -6217,9 +6255,9 @@
       <c r="E48" s="1"/>
     </row>
     <row r="49" spans="1:5" ht="266">
-      <c r="A49" s="33"/>
+      <c r="A49" s="60"/>
       <c r="B49" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C49" s="10" t="s">
         <v>93</v>
@@ -6230,9 +6268,9 @@
       <c r="E49" s="1"/>
     </row>
     <row r="50" spans="1:5" ht="70">
-      <c r="A50" s="33"/>
+      <c r="A50" s="60"/>
       <c r="B50" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C50" s="6" t="s">
         <v>95</v>
@@ -6243,11 +6281,11 @@
       <c r="E50" s="1"/>
     </row>
     <row r="51" spans="1:5" ht="42">
-      <c r="A51" s="33" t="s">
-        <v>158</v>
+      <c r="A51" s="60" t="s">
+        <v>155</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>97</v>
@@ -6258,12 +6296,12 @@
       <c r="E51" s="1"/>
     </row>
     <row r="52" spans="1:5" ht="70">
-      <c r="A52" s="33"/>
+      <c r="A52" s="60"/>
       <c r="B52" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D52" s="4" t="s">
         <v>50</v>
@@ -6271,10 +6309,10 @@
       <c r="E52" s="1"/>
     </row>
     <row r="53" spans="1:5" ht="56">
-      <c r="A53" s="33"/>
+      <c r="A53" s="60"/>
       <c r="B53" s="5"/>
       <c r="C53" s="3" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>51</v>
@@ -6288,7 +6326,7 @@
     <mergeCell ref="A33:A37"/>
     <mergeCell ref="A39:A50"/>
   </mergeCells>
-  <phoneticPr fontId="20" type="noConversion"/>
+  <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" verticalDpi="0"/>
   <headerFooter>

</xml_diff>